<commit_message>
Ajout mise en forme et des données
</commit_message>
<xml_diff>
--- a/doc/avancement Cliiink.xlsx
+++ b/doc/avancement Cliiink.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23408"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\Desktop\cliiink\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D66B8BE-9963-446D-B322-90595770A4DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7507AE8-40DF-40E3-BF47-5514F6D147B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tâches" sheetId="2" r:id="rId1"/>
@@ -4004,8 +4004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53404295-2D02-454B-A260-080633A909F0}">
   <dimension ref="A1:G162"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6687,8 +6687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54278537-4330-487B-8B1E-186EA2F14073}">
   <dimension ref="A1:XFD121"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7361,8 +7361,8 @@
       <c r="H16" s="21"/>
       <c r="I16" s="20"/>
       <c r="J16" s="20"/>
-      <c r="K16" s="54"/>
-      <c r="L16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="54"/>
       <c r="M16" s="21"/>
       <c r="N16" s="21"/>
       <c r="O16" s="21"/>
@@ -7402,7 +7402,7 @@
       <c r="I17" s="20"/>
       <c r="J17" s="20"/>
       <c r="K17" s="43"/>
-      <c r="L17" s="21"/>
+      <c r="L17" s="43"/>
       <c r="M17" s="21"/>
       <c r="N17" s="21"/>
       <c r="O17" s="21"/>
@@ -7442,8 +7442,8 @@
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
       <c r="K18" s="21"/>
-      <c r="L18" s="43"/>
-      <c r="M18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="43"/>
       <c r="N18" s="21"/>
       <c r="O18" s="21"/>
       <c r="P18" s="20"/>
@@ -7483,7 +7483,7 @@
       <c r="J19" s="20"/>
       <c r="K19" s="21"/>
       <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
+      <c r="M19" s="43"/>
       <c r="N19" s="21"/>
       <c r="O19" s="21"/>
       <c r="P19" s="20"/>
@@ -11257,7 +11257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Actualisation avancement + ajout tâche bonus
</commit_message>
<xml_diff>
--- a/doc/avancement Cliiink.xlsx
+++ b/doc/avancement Cliiink.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\Desktop\cliiink\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7507AE8-40DF-40E3-BF47-5514F6D147B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BEDC90-A089-45BD-B96B-53ED6A55B9BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tâches" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="329">
   <si>
     <t>N°</t>
   </si>
@@ -1008,6 +1008,12 @@
   </si>
   <si>
     <t>Avance / Retard (jours-hommes)</t>
+  </si>
+  <si>
+    <t>Gérer les UUID</t>
+  </si>
+  <si>
+    <t>Gérer et enregistrer les UUID comme clés primaires (en format compact) et modifier les requêtes en conséquence</t>
   </si>
 </sst>
 </file>
@@ -1502,7 +1508,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1598,12 +1604,97 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="127">
+  <dxfs count="138">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3567,12 +3658,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{796DFFDF-5600-4057-A29E-6EE432E54146}" name="TachesPrincipales" displayName="TachesPrincipales" ref="A3:G50" totalsRowShown="0">
   <autoFilter ref="A3:G50" xr:uid="{B67725D0-F42F-4B2C-B47E-8586BF5DC6C0}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{6E8FD53C-BEFD-4457-9FA3-9A8A100CC664}" name="N°" dataDxfId="126">
+    <tableColumn id="1" xr3:uid="{6E8FD53C-BEFD-4457-9FA3-9A8A100CC664}" name="N°" dataDxfId="137">
       <calculatedColumnFormula>ROW()-3</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{0069C765-7645-4FD3-9F29-24B7F0C7634C}" name="Tâche"/>
-    <tableColumn id="3" xr3:uid="{A25A25B7-8C3E-419A-9CE3-9FE932DABE3D}" name="Travail (en jours-hommes)" dataDxfId="125"/>
-    <tableColumn id="4" xr3:uid="{A944CAD8-E89F-426E-8FB6-A3FB74D322BE}" name="Tâches requises" dataDxfId="124"/>
+    <tableColumn id="3" xr3:uid="{A25A25B7-8C3E-419A-9CE3-9FE932DABE3D}" name="Travail (en jours-hommes)" dataDxfId="136"/>
+    <tableColumn id="4" xr3:uid="{A944CAD8-E89F-426E-8FB6-A3FB74D322BE}" name="Tâches requises" dataDxfId="135"/>
     <tableColumn id="5" xr3:uid="{A3676B2D-BC63-48C5-A4B6-B4EB56D87918}" name="Objectifs"/>
     <tableColumn id="6" xr3:uid="{01DF4278-05CC-4D78-B336-D2F095AF927E}" name="Critères d’achèvement"/>
     <tableColumn id="7" xr3:uid="{99493734-498F-43D2-92ED-EAA3DB0F4B00}" name="Livrables"/>
@@ -3582,15 +3673,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9F70FDBF-93E5-4529-8B86-C46B44C9F1C9}" name="TachesBonus" displayName="TachesBonus" ref="A52:G108" totalsRowShown="0" headerRowDxfId="123" headerRowBorderDxfId="122" tableBorderDxfId="121">
-  <autoFilter ref="A52:G108" xr:uid="{6375B6D4-F047-429E-A127-A4478080FC25}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9F70FDBF-93E5-4529-8B86-C46B44C9F1C9}" name="TachesBonus" displayName="TachesBonus" ref="A52:G109" totalsRowShown="0" headerRowDxfId="134" headerRowBorderDxfId="133" tableBorderDxfId="132">
+  <autoFilter ref="A52:G109" xr:uid="{6375B6D4-F047-429E-A127-A4478080FC25}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{6333C598-AB08-4105-92D3-D88D2B08DCCB}" name="N°" dataDxfId="120">
+    <tableColumn id="1" xr3:uid="{6333C598-AB08-4105-92D3-D88D2B08DCCB}" name="N°" dataDxfId="131">
       <calculatedColumnFormula>ROW()-5</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{53B86B66-0396-4D8B-B984-B80A4F587612}" name="Tâche"/>
-    <tableColumn id="3" xr3:uid="{D23D171C-1F80-4C5B-B986-46C3CCC8AE38}" name="Travail (en jours-hommes)" dataDxfId="119"/>
-    <tableColumn id="4" xr3:uid="{E0E75BF9-64EA-4FE8-90E4-1AAA1CED01EF}" name="Tâches requises" dataDxfId="118"/>
+    <tableColumn id="3" xr3:uid="{D23D171C-1F80-4C5B-B986-46C3CCC8AE38}" name="Travail (en jours-hommes)" dataDxfId="130"/>
+    <tableColumn id="4" xr3:uid="{E0E75BF9-64EA-4FE8-90E4-1AAA1CED01EF}" name="Tâches requises" dataDxfId="129"/>
     <tableColumn id="5" xr3:uid="{78EA56D9-206B-4896-BDD8-ECE5895F3943}" name="Objectifs"/>
     <tableColumn id="6" xr3:uid="{537B5B27-0138-4B69-AACD-BA754420310A}" name="Critères d’achèvement"/>
     <tableColumn id="7" xr3:uid="{F5B2842E-F201-4E20-BBB3-296B792E130C}" name="Livrables"/>
@@ -3600,140 +3691,140 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E08C3540-563F-4309-961F-3A2D48BF908C}" name="PlanningPrincipal" displayName="PlanningPrincipal" ref="A4:AD51" headerRowDxfId="117">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E08C3540-563F-4309-961F-3A2D48BF908C}" name="PlanningPrincipal" displayName="PlanningPrincipal" ref="A4:AD51" headerRowDxfId="128">
   <autoFilter ref="A4:AD51" xr:uid="{3869585A-DD74-4715-8B08-BD2783F0B46B}"/>
   <tableColumns count="30">
-    <tableColumn id="31" xr3:uid="{02974BA7-1E46-4150-A100-3503892E7F24}" name="N°" dataDxfId="116" totalsRowDxfId="115">
+    <tableColumn id="31" xr3:uid="{02974BA7-1E46-4150-A100-3503892E7F24}" name="N°" dataDxfId="127" totalsRowDxfId="126">
       <calculatedColumnFormula>Tâches!A4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="1" xr3:uid="{B537D5E3-048F-47B6-A4D3-4925E570D546}" name="Type" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{9B7DC595-B3F0-4BA6-A2B3-7B3F96E6422C}" name="Tâche" dataDxfId="114" totalsRowDxfId="113">
+    <tableColumn id="2" xr3:uid="{9B7DC595-B3F0-4BA6-A2B3-7B3F96E6422C}" name="Tâche" dataDxfId="125" totalsRowDxfId="124">
       <calculatedColumnFormula>Tâches!B4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{7CF5EF96-F7EA-4081-A9F6-C6030E29374A}" name="05-oct" dataDxfId="112" totalsRowDxfId="111"/>
-    <tableColumn id="4" xr3:uid="{AED08872-92A3-48EC-9686-65D32A38B01C}" name="06-oct" dataDxfId="110" totalsRowDxfId="109"/>
-    <tableColumn id="5" xr3:uid="{A361D231-81F6-4E0E-9D68-F198542EC510}" name="07-oct" dataDxfId="108" totalsRowDxfId="107"/>
-    <tableColumn id="6" xr3:uid="{95C7985A-0503-4B82-A39B-7087B64C463E}" name="08-oct" dataDxfId="106" totalsRowDxfId="105"/>
-    <tableColumn id="7" xr3:uid="{223BBA38-BBF5-4596-9520-B3C80EF77B2C}" name="09-oct" dataDxfId="104" totalsRowDxfId="103"/>
-    <tableColumn id="8" xr3:uid="{CBA2CED5-BFCD-478D-BC0B-64F7236665B8}" name="10-oct" dataDxfId="102" totalsRowDxfId="101"/>
-    <tableColumn id="9" xr3:uid="{9142E539-6B94-44F9-AE32-D9D0257404D4}" name="11-oct" dataDxfId="100" totalsRowDxfId="99"/>
-    <tableColumn id="10" xr3:uid="{3DF50CC7-E072-416C-9E4D-77F99E3AFEE4}" name="12-oct" dataDxfId="98" totalsRowDxfId="97"/>
-    <tableColumn id="11" xr3:uid="{1BA6AA9C-31C1-4DF3-AB9B-EE58F953EA7B}" name="13-oct" dataDxfId="96" totalsRowDxfId="95"/>
-    <tableColumn id="12" xr3:uid="{E3903BB0-7B8A-45F4-8E32-0DEC3020D2C7}" name="14-oct" dataDxfId="94" totalsRowDxfId="93"/>
-    <tableColumn id="13" xr3:uid="{902C3056-E350-4CB3-8791-82ADD700A68A}" name="15-oct" dataDxfId="92" totalsRowDxfId="91"/>
-    <tableColumn id="14" xr3:uid="{54609321-2FA1-4A62-830E-30F3A492893D}" name="16-oct" dataDxfId="90" totalsRowDxfId="89"/>
-    <tableColumn id="15" xr3:uid="{3F1B4408-EFA2-430D-89AE-07B73C0F975A}" name="17-oct" dataDxfId="88" totalsRowDxfId="87"/>
-    <tableColumn id="16" xr3:uid="{6DC91AA7-F87C-4075-9A2A-AF1EB7BCC95B}" name="18-oct" dataDxfId="86" totalsRowDxfId="85"/>
-    <tableColumn id="17" xr3:uid="{0AA6E344-3437-43D3-992F-24D8117454B9}" name="19-oct" dataDxfId="84" totalsRowDxfId="83"/>
-    <tableColumn id="18" xr3:uid="{96D8D6A9-008E-484B-B7B4-28ABA94491F0}" name="20-oct" dataDxfId="82" totalsRowDxfId="81"/>
-    <tableColumn id="19" xr3:uid="{C6993608-949D-47F9-B239-5455810AAC64}" name="21-oct" dataDxfId="80" totalsRowDxfId="79"/>
-    <tableColumn id="20" xr3:uid="{D1F65972-7A93-4F3D-9DD9-0066440F9CD3}" name="22-oct" dataDxfId="78" totalsRowDxfId="77"/>
-    <tableColumn id="21" xr3:uid="{2491BABE-5995-4D9B-9106-2E6B37978835}" name="23-oct" dataDxfId="76" totalsRowDxfId="75"/>
-    <tableColumn id="22" xr3:uid="{AFD0F5C6-D453-44A7-A7A2-E80250827459}" name="24-oct" dataDxfId="74" totalsRowDxfId="73"/>
-    <tableColumn id="23" xr3:uid="{05DEBB6A-759F-4C9F-AF39-B31DA26929B5}" name="25-oct" dataDxfId="72" totalsRowDxfId="71"/>
-    <tableColumn id="24" xr3:uid="{0F14F7F0-8C7B-47D9-A425-10B6AB326102}" name="26-oct" dataDxfId="70" totalsRowDxfId="69"/>
-    <tableColumn id="25" xr3:uid="{F63019F4-1021-4A1C-AD12-1FA5B5EAC831}" name="27-oct" dataDxfId="68" totalsRowDxfId="67"/>
-    <tableColumn id="26" xr3:uid="{A0FA9325-6D8A-4E3F-841E-0A51A69AA21F}" name="28-oct" dataDxfId="66" totalsRowDxfId="65"/>
-    <tableColumn id="27" xr3:uid="{01390279-2B86-4CDA-AACC-12D48EE68027}" name="29-oct" dataDxfId="64" totalsRowDxfId="63"/>
-    <tableColumn id="28" xr3:uid="{9E31ED4A-02CE-4F4A-8A83-5681191E9E9E}" name="30-oct" dataDxfId="62" totalsRowDxfId="61"/>
-    <tableColumn id="29" xr3:uid="{885B064E-7B13-4C56-B53C-04028C7E7B19}" name="31-oct" totalsRowFunction="count" dataDxfId="60" totalsRowDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{7CF5EF96-F7EA-4081-A9F6-C6030E29374A}" name="05-oct" dataDxfId="123" totalsRowDxfId="122"/>
+    <tableColumn id="4" xr3:uid="{AED08872-92A3-48EC-9686-65D32A38B01C}" name="06-oct" dataDxfId="121" totalsRowDxfId="120"/>
+    <tableColumn id="5" xr3:uid="{A361D231-81F6-4E0E-9D68-F198542EC510}" name="07-oct" dataDxfId="119" totalsRowDxfId="118"/>
+    <tableColumn id="6" xr3:uid="{95C7985A-0503-4B82-A39B-7087B64C463E}" name="08-oct" dataDxfId="117" totalsRowDxfId="116"/>
+    <tableColumn id="7" xr3:uid="{223BBA38-BBF5-4596-9520-B3C80EF77B2C}" name="09-oct" dataDxfId="115" totalsRowDxfId="114"/>
+    <tableColumn id="8" xr3:uid="{CBA2CED5-BFCD-478D-BC0B-64F7236665B8}" name="10-oct" dataDxfId="113" totalsRowDxfId="112"/>
+    <tableColumn id="9" xr3:uid="{9142E539-6B94-44F9-AE32-D9D0257404D4}" name="11-oct" dataDxfId="111" totalsRowDxfId="110"/>
+    <tableColumn id="10" xr3:uid="{3DF50CC7-E072-416C-9E4D-77F99E3AFEE4}" name="12-oct" dataDxfId="109" totalsRowDxfId="108"/>
+    <tableColumn id="11" xr3:uid="{1BA6AA9C-31C1-4DF3-AB9B-EE58F953EA7B}" name="13-oct" dataDxfId="107" totalsRowDxfId="106"/>
+    <tableColumn id="12" xr3:uid="{E3903BB0-7B8A-45F4-8E32-0DEC3020D2C7}" name="14-oct" dataDxfId="105" totalsRowDxfId="104"/>
+    <tableColumn id="13" xr3:uid="{902C3056-E350-4CB3-8791-82ADD700A68A}" name="15-oct" dataDxfId="103" totalsRowDxfId="102"/>
+    <tableColumn id="14" xr3:uid="{54609321-2FA1-4A62-830E-30F3A492893D}" name="16-oct" dataDxfId="101" totalsRowDxfId="100"/>
+    <tableColumn id="15" xr3:uid="{3F1B4408-EFA2-430D-89AE-07B73C0F975A}" name="17-oct" dataDxfId="99" totalsRowDxfId="98"/>
+    <tableColumn id="16" xr3:uid="{6DC91AA7-F87C-4075-9A2A-AF1EB7BCC95B}" name="18-oct" dataDxfId="97" totalsRowDxfId="96"/>
+    <tableColumn id="17" xr3:uid="{0AA6E344-3437-43D3-992F-24D8117454B9}" name="19-oct" dataDxfId="95" totalsRowDxfId="94"/>
+    <tableColumn id="18" xr3:uid="{96D8D6A9-008E-484B-B7B4-28ABA94491F0}" name="20-oct" dataDxfId="93" totalsRowDxfId="92"/>
+    <tableColumn id="19" xr3:uid="{C6993608-949D-47F9-B239-5455810AAC64}" name="21-oct" dataDxfId="91" totalsRowDxfId="90"/>
+    <tableColumn id="20" xr3:uid="{D1F65972-7A93-4F3D-9DD9-0066440F9CD3}" name="22-oct" dataDxfId="89" totalsRowDxfId="88"/>
+    <tableColumn id="21" xr3:uid="{2491BABE-5995-4D9B-9106-2E6B37978835}" name="23-oct" dataDxfId="87" totalsRowDxfId="86"/>
+    <tableColumn id="22" xr3:uid="{AFD0F5C6-D453-44A7-A7A2-E80250827459}" name="24-oct" dataDxfId="85" totalsRowDxfId="84"/>
+    <tableColumn id="23" xr3:uid="{05DEBB6A-759F-4C9F-AF39-B31DA26929B5}" name="25-oct" dataDxfId="83" totalsRowDxfId="82"/>
+    <tableColumn id="24" xr3:uid="{0F14F7F0-8C7B-47D9-A425-10B6AB326102}" name="26-oct" dataDxfId="81" totalsRowDxfId="80"/>
+    <tableColumn id="25" xr3:uid="{F63019F4-1021-4A1C-AD12-1FA5B5EAC831}" name="27-oct" dataDxfId="79" totalsRowDxfId="78"/>
+    <tableColumn id="26" xr3:uid="{A0FA9325-6D8A-4E3F-841E-0A51A69AA21F}" name="28-oct" dataDxfId="77" totalsRowDxfId="76"/>
+    <tableColumn id="27" xr3:uid="{01390279-2B86-4CDA-AACC-12D48EE68027}" name="29-oct" dataDxfId="75" totalsRowDxfId="74"/>
+    <tableColumn id="28" xr3:uid="{9E31ED4A-02CE-4F4A-8A83-5681191E9E9E}" name="30-oct" dataDxfId="73" totalsRowDxfId="72"/>
+    <tableColumn id="29" xr3:uid="{885B064E-7B13-4C56-B53C-04028C7E7B19}" name="31-oct" totalsRowFunction="count" dataDxfId="71" totalsRowDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{949F634D-FB76-42BC-8AD2-845CBF052EB4}" name="PlanningBonus" displayName="PlanningBonus" ref="A54:AD110" totalsRowShown="0" headerRowDxfId="58">
-  <autoFilter ref="A54:AD110" xr:uid="{C72AC31B-BC16-4ED0-A742-6FDD0EBB8631}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{949F634D-FB76-42BC-8AD2-845CBF052EB4}" name="PlanningBonus" displayName="PlanningBonus" ref="A54:AD111" totalsRowShown="0" headerRowDxfId="69">
+  <autoFilter ref="A54:AD111" xr:uid="{C72AC31B-BC16-4ED0-A742-6FDD0EBB8631}"/>
   <tableColumns count="30">
-    <tableColumn id="30" xr3:uid="{A9929115-DAFC-40AE-A75F-89D94A3A6E3E}" name="N°" dataDxfId="57">
+    <tableColumn id="30" xr3:uid="{A9929115-DAFC-40AE-A75F-89D94A3A6E3E}" name="N°" dataDxfId="68">
       <calculatedColumnFormula>Tâches!A53</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="1" xr3:uid="{D9389245-51FF-4B4C-8D41-B0C82DF9FA75}" name="Type"/>
-    <tableColumn id="2" xr3:uid="{725C423E-FCC3-4D2B-A7B1-04718A631379}" name="Tâche" dataDxfId="56">
-      <calculatedColumnFormula>Tâches!B53</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{725C423E-FCC3-4D2B-A7B1-04718A631379}" name="Tâche" dataDxfId="67">
+      <calculatedColumnFormula>Tâches!B54</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{3E9DBF51-63AA-41C7-8026-17B53B0A9B6C}" name="05-oct" dataDxfId="55"/>
-    <tableColumn id="4" xr3:uid="{82D5CCDD-F94F-4AD0-87E3-71A24CD87405}" name="06-oct" dataDxfId="54"/>
-    <tableColumn id="5" xr3:uid="{BE2F3F2A-9776-4093-805A-312DDC6F80FE}" name="07-oct" dataDxfId="53"/>
-    <tableColumn id="6" xr3:uid="{C1BB4810-F8A8-4B1C-BEFF-BCD91A7CBE63}" name="08-oct" dataDxfId="52"/>
-    <tableColumn id="7" xr3:uid="{81533870-EEB5-4296-AE2B-E1E0C4B449EA}" name="09-oct" dataDxfId="51"/>
-    <tableColumn id="8" xr3:uid="{5614AF65-2E97-4A81-93F3-4BF71D68BA64}" name="10-oct" dataDxfId="50"/>
-    <tableColumn id="9" xr3:uid="{68ABF0CA-AF48-4143-8348-D852DD541BEA}" name="11-oct" dataDxfId="49"/>
-    <tableColumn id="10" xr3:uid="{D00B30BB-B608-47A8-A909-B3CCE0CD31F7}" name="12-oct" dataDxfId="48"/>
-    <tableColumn id="11" xr3:uid="{E0989A06-4A1E-4309-B9D8-FFF15CEF945C}" name="13-oct" dataDxfId="47"/>
-    <tableColumn id="12" xr3:uid="{1779F27B-A65D-4938-A036-4979FC026FF9}" name="14-oct" dataDxfId="46"/>
-    <tableColumn id="13" xr3:uid="{22F38C55-7716-4548-902D-BF65239896B9}" name="15-oct" dataDxfId="45"/>
-    <tableColumn id="14" xr3:uid="{0379C43C-369A-4D33-98C8-09F6AB1138A5}" name="16-oct" dataDxfId="44"/>
-    <tableColumn id="15" xr3:uid="{95071E30-9EB4-4F6F-863F-5DDBD2FC2727}" name="17-oct" dataDxfId="43"/>
-    <tableColumn id="16" xr3:uid="{57019D85-E364-4C2A-8EDF-EECF1621D7F4}" name="18-oct" dataDxfId="42"/>
-    <tableColumn id="17" xr3:uid="{E1AB2C2B-7642-4E82-9C5D-D1EBE0244AAA}" name="19-oct" dataDxfId="41"/>
-    <tableColumn id="18" xr3:uid="{109FE92E-C236-400D-8A95-114BD055E9DA}" name="20-oct" dataDxfId="40"/>
-    <tableColumn id="19" xr3:uid="{F53D6821-A790-4CAC-82E2-E3B0BA8021AD}" name="21-oct" dataDxfId="39"/>
-    <tableColumn id="20" xr3:uid="{E29FFFEE-7FB8-414D-BCCD-0CBC972A8026}" name="22-oct" dataDxfId="38"/>
-    <tableColumn id="21" xr3:uid="{143958D3-765B-428D-A750-762564AFF52B}" name="23-oct" dataDxfId="37"/>
-    <tableColumn id="22" xr3:uid="{F6E67B4D-280E-47A5-AF79-5FF172D2E5C7}" name="24-oct" dataDxfId="36"/>
-    <tableColumn id="23" xr3:uid="{A16D3DC4-7696-40A7-8B9F-1454BEC9DBC2}" name="25-oct" dataDxfId="35"/>
-    <tableColumn id="24" xr3:uid="{218180A7-E150-4120-8AE9-6723F56E1D9B}" name="26-oct" dataDxfId="34"/>
-    <tableColumn id="25" xr3:uid="{AFF74DA3-B552-40C8-A8FE-1E5490C0DC0B}" name="27-oct" dataDxfId="33"/>
-    <tableColumn id="26" xr3:uid="{38E7E763-F0C2-4BFE-A84B-1E26140C2250}" name="28-oct" dataDxfId="32"/>
-    <tableColumn id="27" xr3:uid="{988E4DC2-CA0F-4098-B08C-759F208CFD2A}" name="29-oct" dataDxfId="31"/>
-    <tableColumn id="28" xr3:uid="{539EA04B-D1E5-47FC-9E69-E37BB7704D5C}" name="30-oct" dataDxfId="30"/>
-    <tableColumn id="29" xr3:uid="{21E9E5C4-8D23-454B-8A91-1CF8DA5078B0}" name="31-oct" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{3E9DBF51-63AA-41C7-8026-17B53B0A9B6C}" name="05-oct" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{82D5CCDD-F94F-4AD0-87E3-71A24CD87405}" name="06-oct" dataDxfId="65"/>
+    <tableColumn id="5" xr3:uid="{BE2F3F2A-9776-4093-805A-312DDC6F80FE}" name="07-oct" dataDxfId="64"/>
+    <tableColumn id="6" xr3:uid="{C1BB4810-F8A8-4B1C-BEFF-BCD91A7CBE63}" name="08-oct" dataDxfId="63"/>
+    <tableColumn id="7" xr3:uid="{81533870-EEB5-4296-AE2B-E1E0C4B449EA}" name="09-oct" dataDxfId="62"/>
+    <tableColumn id="8" xr3:uid="{5614AF65-2E97-4A81-93F3-4BF71D68BA64}" name="10-oct" dataDxfId="61"/>
+    <tableColumn id="9" xr3:uid="{68ABF0CA-AF48-4143-8348-D852DD541BEA}" name="11-oct" dataDxfId="60"/>
+    <tableColumn id="10" xr3:uid="{D00B30BB-B608-47A8-A909-B3CCE0CD31F7}" name="12-oct" dataDxfId="59"/>
+    <tableColumn id="11" xr3:uid="{E0989A06-4A1E-4309-B9D8-FFF15CEF945C}" name="13-oct" dataDxfId="58"/>
+    <tableColumn id="12" xr3:uid="{1779F27B-A65D-4938-A036-4979FC026FF9}" name="14-oct" dataDxfId="57"/>
+    <tableColumn id="13" xr3:uid="{22F38C55-7716-4548-902D-BF65239896B9}" name="15-oct" dataDxfId="56"/>
+    <tableColumn id="14" xr3:uid="{0379C43C-369A-4D33-98C8-09F6AB1138A5}" name="16-oct" dataDxfId="55"/>
+    <tableColumn id="15" xr3:uid="{95071E30-9EB4-4F6F-863F-5DDBD2FC2727}" name="17-oct" dataDxfId="54"/>
+    <tableColumn id="16" xr3:uid="{57019D85-E364-4C2A-8EDF-EECF1621D7F4}" name="18-oct" dataDxfId="53"/>
+    <tableColumn id="17" xr3:uid="{E1AB2C2B-7642-4E82-9C5D-D1EBE0244AAA}" name="19-oct" dataDxfId="52"/>
+    <tableColumn id="18" xr3:uid="{109FE92E-C236-400D-8A95-114BD055E9DA}" name="20-oct" dataDxfId="51"/>
+    <tableColumn id="19" xr3:uid="{F53D6821-A790-4CAC-82E2-E3B0BA8021AD}" name="21-oct" dataDxfId="50"/>
+    <tableColumn id="20" xr3:uid="{E29FFFEE-7FB8-414D-BCCD-0CBC972A8026}" name="22-oct" dataDxfId="49"/>
+    <tableColumn id="21" xr3:uid="{143958D3-765B-428D-A750-762564AFF52B}" name="23-oct" dataDxfId="48"/>
+    <tableColumn id="22" xr3:uid="{F6E67B4D-280E-47A5-AF79-5FF172D2E5C7}" name="24-oct" dataDxfId="47"/>
+    <tableColumn id="23" xr3:uid="{A16D3DC4-7696-40A7-8B9F-1454BEC9DBC2}" name="25-oct" dataDxfId="46"/>
+    <tableColumn id="24" xr3:uid="{218180A7-E150-4120-8AE9-6723F56E1D9B}" name="26-oct" dataDxfId="45"/>
+    <tableColumn id="25" xr3:uid="{AFF74DA3-B552-40C8-A8FE-1E5490C0DC0B}" name="27-oct" dataDxfId="44"/>
+    <tableColumn id="26" xr3:uid="{38E7E763-F0C2-4BFE-A84B-1E26140C2250}" name="28-oct" dataDxfId="43"/>
+    <tableColumn id="27" xr3:uid="{988E4DC2-CA0F-4098-B08C-759F208CFD2A}" name="29-oct" dataDxfId="42"/>
+    <tableColumn id="28" xr3:uid="{539EA04B-D1E5-47FC-9E69-E37BB7704D5C}" name="30-oct" dataDxfId="41"/>
+    <tableColumn id="29" xr3:uid="{21E9E5C4-8D23-454B-8A91-1CF8DA5078B0}" name="31-oct" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0DEB2AD8-CEC3-48AA-9CF7-ED08DF8D0180}" name="AvancementPrincipal" displayName="AvancementPrincipal" ref="A3:H50" totalsRowShown="0" headerRowDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0DEB2AD8-CEC3-48AA-9CF7-ED08DF8D0180}" name="AvancementPrincipal" displayName="AvancementPrincipal" ref="A3:H50" totalsRowShown="0" headerRowDxfId="39">
   <autoFilter ref="A3:H50" xr:uid="{6BCE8A7D-7D04-4394-AD53-9D2B48AA6CFD}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B07E0580-F8B1-4A81-8EA6-8D0DD94E6CBF}" name="N°" dataDxfId="27">
+    <tableColumn id="1" xr3:uid="{B07E0580-F8B1-4A81-8EA6-8D0DD94E6CBF}" name="N°" dataDxfId="38">
       <calculatedColumnFormula>TachesPrincipales[[#This Row],[N°]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{CD2C34A8-4A66-4D31-8674-72875FEEBCB9}" name="Tâche" dataDxfId="26">
+    <tableColumn id="2" xr3:uid="{CD2C34A8-4A66-4D31-8674-72875FEEBCB9}" name="Tâche" dataDxfId="37">
       <calculatedColumnFormula>TachesPrincipales[[#This Row],[Tâche]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1F692755-0EBF-47B3-98F7-5870DAAA2B47}" name="Durée estimée (jours-hommes)" dataDxfId="25">
+    <tableColumn id="3" xr3:uid="{1F692755-0EBF-47B3-98F7-5870DAAA2B47}" name="Durée estimée (jours-hommes)" dataDxfId="36">
       <calculatedColumnFormula>TachesPrincipales[[#This Row],[Travail (en jours-hommes)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77A08BA6-0C47-4CA1-898D-34688079E99A}" name="Temps consacré (jours-hommes)" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{E6DFF25A-5C0F-4D2B-AD4B-356CCC3C697D}" name="Temps restant (jours-hommes)" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{80B25DCD-7C24-4853-87D7-112B68A75ACA}" name="Complétion" dataDxfId="22">
+    <tableColumn id="4" xr3:uid="{77A08BA6-0C47-4CA1-898D-34688079E99A}" name="Temps consacré (jours-hommes)" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{E6DFF25A-5C0F-4D2B-AD4B-356CCC3C697D}" name="Temps restant (jours-hommes)" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{80B25DCD-7C24-4853-87D7-112B68A75ACA}" name="Complétion" dataDxfId="33">
       <calculatedColumnFormula>IFERROR(AvancementPrincipal[[#This Row],[Temps consacré (jours-hommes)]]/(AvancementPrincipal[[#This Row],[Temps consacré (jours-hommes)]]+AvancementPrincipal[[#This Row],[Temps restant (jours-hommes)]]), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E98F81A4-15B7-43AA-8EE6-E47F2F7BDDBA}" name="Avance / Retard (jours-hommes)" dataDxfId="21">
+    <tableColumn id="9" xr3:uid="{E98F81A4-15B7-43AA-8EE6-E47F2F7BDDBA}" name="Avance / Retard (jours-hommes)" dataDxfId="32">
       <calculatedColumnFormula>IF(AvancementPrincipal[[#This Row],[Temps consacré (jours-hommes)]]&lt;&gt;"",AvancementPrincipal[[#This Row],[Durée estimée (jours-hommes)]]-AvancementPrincipal[[#This Row],[Temps consacré (jours-hommes)]]-AvancementPrincipal[[#This Row],[Temps restant (jours-hommes)]],"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{19DBC3BA-BFF6-4123-B35C-1B58A7832A4B}" name="Commentaire" dataDxfId="20" dataCellStyle="Percent"/>
+    <tableColumn id="7" xr3:uid="{19DBC3BA-BFF6-4123-B35C-1B58A7832A4B}" name="Commentaire" dataDxfId="31" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{04BF9D35-9277-48A6-B974-1A1D7A80EEAE}" name="AvancementPrincipal8" displayName="AvancementPrincipal8" ref="A52:H108" totalsRowShown="0" headerRowDxfId="19">
-  <autoFilter ref="A52:H108" xr:uid="{43FC80CF-67C7-44CB-8AF9-C483360ED027}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{04BF9D35-9277-48A6-B974-1A1D7A80EEAE}" name="AvancementPrincipal8" displayName="AvancementPrincipal8" ref="A52:H109" totalsRowShown="0" headerRowDxfId="30">
+  <autoFilter ref="A52:H109" xr:uid="{43FC80CF-67C7-44CB-8AF9-C483360ED027}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{50AEF074-CE1B-4E86-81E2-68DBB744C39B}" name="N°" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{50AEF074-CE1B-4E86-81E2-68DBB744C39B}" name="N°" dataDxfId="29">
       <calculatedColumnFormula>TachesBonus[[#This Row],[N°]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{23C870F0-9110-4D2F-8665-88DA3D2D1265}" name="Tâche" dataDxfId="17">
+    <tableColumn id="2" xr3:uid="{23C870F0-9110-4D2F-8665-88DA3D2D1265}" name="Tâche" dataDxfId="28">
       <calculatedColumnFormula>TachesBonus[[#This Row],[Tâche]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{69BB17CC-DE87-420A-BBFA-062BF2BEF7AA}" name="Durée estimée (jours-hommes)" dataDxfId="16">
+    <tableColumn id="3" xr3:uid="{69BB17CC-DE87-420A-BBFA-062BF2BEF7AA}" name="Durée estimée (jours-hommes)" dataDxfId="27">
       <calculatedColumnFormula>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A14AEF2F-CFF6-4D95-9EB5-0A11BA283D4F}" name="Temps consacré (jours-hommes)" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{25E0D910-E053-4859-9A05-DA9FEEB0AC2A}" name="Temps restant (jours-hommes)" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{5E4CFA2C-63BF-45F7-9435-50DEBD5B0D2E}" name="Complétion" dataDxfId="13">
+    <tableColumn id="4" xr3:uid="{A14AEF2F-CFF6-4D95-9EB5-0A11BA283D4F}" name="Temps consacré (jours-hommes)" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{25E0D910-E053-4859-9A05-DA9FEEB0AC2A}" name="Temps restant (jours-hommes)" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{5E4CFA2C-63BF-45F7-9435-50DEBD5B0D2E}" name="Complétion" dataDxfId="24">
       <calculatedColumnFormula>IFERROR(AvancementPrincipal8[[#This Row],[Temps consacré (jours-hommes)]]/(AvancementPrincipal8[[#This Row],[Temps consacré (jours-hommes)]]+AvancementPrincipal8[[#This Row],[Temps restant (jours-hommes)]]), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{B0B94A9D-C385-47C1-9326-CF1085FB5FB7}" name="Avance / Retard (jours-hommes)" dataDxfId="12">
+    <tableColumn id="9" xr3:uid="{B0B94A9D-C385-47C1-9326-CF1085FB5FB7}" name="Avance / Retard (jours-hommes)" dataDxfId="23">
       <calculatedColumnFormula>IF(AvancementPrincipal8[[#This Row],[Temps consacré (jours-hommes)]]&lt;&gt;"",AvancementPrincipal8[[#This Row],[Durée estimée (jours-hommes)]]-AvancementPrincipal8[[#This Row],[Temps consacré (jours-hommes)]]-AvancementPrincipal8[[#This Row],[Temps restant (jours-hommes)]],"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3B743E05-8FA8-4C6C-91C3-7DC6C79CF839}" name="Commentaire" dataDxfId="11" dataCellStyle="Percent"/>
+    <tableColumn id="7" xr3:uid="{3B743E05-8FA8-4C6C-91C3-7DC6C79CF839}" name="Commentaire" dataDxfId="22" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4002,10 +4093,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53404295-2D02-454B-A260-080633A909F0}">
-  <dimension ref="A1:G162"/>
+  <dimension ref="A1:G163"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5212,48 +5303,47 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
-        <f t="shared" ref="A53:A98" si="4">ROW()-5</f>
+        <f t="shared" ref="A53:A99" si="4">ROW()-5</f>
         <v>48</v>
       </c>
       <c r="B53" t="s">
+        <v>327</v>
+      </c>
+      <c r="C53" s="14">
+        <v>2</v>
+      </c>
+      <c r="D53" s="5">
+        <v>16</v>
+      </c>
+      <c r="E53" t="s">
+        <v>328</v>
+      </c>
+      <c r="F53" t="s">
+        <v>24</v>
+      </c>
+      <c r="G53" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="66">
+        <f>ROW()-5</f>
+        <v>49</v>
+      </c>
+      <c r="B54" t="s">
         <v>138</v>
       </c>
-      <c r="C53" s="14">
-        <v>1</v>
-      </c>
-      <c r="E53" t="s">
+      <c r="C54" s="14">
+        <v>1</v>
+      </c>
+      <c r="E54" t="s">
         <v>70</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F54" t="s">
         <v>216</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G54" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="8">
-        <f t="shared" si="4"/>
-        <v>49</v>
-      </c>
-      <c r="B54" t="s">
-        <v>163</v>
-      </c>
-      <c r="C54" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="D54" s="5">
-        <f>A53</f>
-        <v>48</v>
-      </c>
-      <c r="E54" t="s">
-        <v>7</v>
-      </c>
-      <c r="F54" t="s">
-        <v>8</v>
-      </c>
-      <c r="G54" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -5262,23 +5352,23 @@
         <v>50</v>
       </c>
       <c r="B55" t="s">
-        <v>139</v>
+        <v>163</v>
       </c>
       <c r="C55" s="14">
         <v>0.5</v>
       </c>
       <c r="D55" s="5">
-        <f t="shared" ref="D55:D58" si="5">A54</f>
-        <v>49</v>
+        <f>A53</f>
+        <v>48</v>
       </c>
       <c r="E55" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F55" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G55" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -5287,20 +5377,20 @@
         <v>51</v>
       </c>
       <c r="B56" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C56" s="14">
         <v>0.5</v>
       </c>
       <c r="D56" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="D56:D59" si="5">A55</f>
         <v>50</v>
       </c>
       <c r="E56" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F56" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G56" t="s">
         <v>12</v>
@@ -5312,7 +5402,7 @@
         <v>52</v>
       </c>
       <c r="B57" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C57" s="14">
         <v>0.5</v>
@@ -5322,10 +5412,10 @@
         <v>51</v>
       </c>
       <c r="E57" t="s">
-        <v>200</v>
+        <v>13</v>
       </c>
       <c r="F57" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G57" t="s">
         <v>12</v>
@@ -5337,23 +5427,23 @@
         <v>53</v>
       </c>
       <c r="B58" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C58" s="14">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D58" s="5">
         <f t="shared" si="5"/>
         <v>52</v>
       </c>
       <c r="E58" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F58" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G58" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -5362,19 +5452,23 @@
         <v>54</v>
       </c>
       <c r="B59" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C59" s="14">
         <v>1</v>
       </c>
+      <c r="D59" s="5">
+        <f t="shared" si="5"/>
+        <v>53</v>
+      </c>
       <c r="E59" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="F59" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G59" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -5383,19 +5477,16 @@
         <v>55</v>
       </c>
       <c r="B60" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C60" s="14">
         <v>1</v>
       </c>
-      <c r="D60" s="5" t="s">
-        <v>258</v>
-      </c>
       <c r="E60" t="s">
-        <v>53</v>
+        <v>201</v>
       </c>
       <c r="F60" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G60" t="s">
         <v>6</v>
@@ -5407,20 +5498,19 @@
         <v>56</v>
       </c>
       <c r="B61" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C61" s="14">
         <v>1</v>
       </c>
-      <c r="D61" s="5">
-        <f>A60</f>
-        <v>55</v>
+      <c r="D61" s="5" t="s">
+        <v>258</v>
       </c>
       <c r="E61" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="F61" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G61" t="s">
         <v>6</v>
@@ -5432,23 +5522,23 @@
         <v>57</v>
       </c>
       <c r="B62" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C62" s="14">
         <v>1</v>
       </c>
       <c r="D62" s="5">
-        <f>A58</f>
-        <v>53</v>
+        <f>A61</f>
+        <v>56</v>
       </c>
       <c r="E62" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F62" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G62" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -5457,23 +5547,23 @@
         <v>58</v>
       </c>
       <c r="B63" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="C63" s="14">
         <v>1</v>
       </c>
       <c r="D63" s="5">
-        <f>A62</f>
-        <v>57</v>
+        <f>A59</f>
+        <v>54</v>
       </c>
       <c r="E63" t="s">
-        <v>204</v>
+        <v>23</v>
       </c>
       <c r="F63" t="s">
-        <v>218</v>
+        <v>24</v>
       </c>
       <c r="G63" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -5482,46 +5572,47 @@
         <v>59</v>
       </c>
       <c r="B64" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C64" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>260</v>
+        <v>1</v>
+      </c>
+      <c r="D64" s="5">
+        <f>A63</f>
+        <v>58</v>
       </c>
       <c r="E64" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="F64" t="s">
-        <v>29</v>
+        <v>218</v>
       </c>
       <c r="G64" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="8">
-        <f>ROW()-5</f>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="B65" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C65" s="14">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E65" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F65" t="s">
-        <v>220</v>
+        <v>29</v>
       </c>
       <c r="G65" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -5530,16 +5621,16 @@
         <v>61</v>
       </c>
       <c r="B66" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C66" s="14">
         <v>1</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E66" t="s">
-        <v>205</v>
+        <v>230</v>
       </c>
       <c r="F66" t="s">
         <v>220</v>
@@ -5550,26 +5641,26 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="8">
-        <f t="shared" si="4"/>
+        <f>ROW()-5</f>
         <v>62</v>
       </c>
       <c r="B67" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C67" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="E67" t="s">
-        <v>231</v>
+        <v>205</v>
       </c>
       <c r="F67" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G67" t="s">
-        <v>76</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -5578,19 +5669,22 @@
         <v>63</v>
       </c>
       <c r="B68" t="s">
-        <v>128</v>
+        <v>168</v>
       </c>
       <c r="C68" s="14">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>262</v>
       </c>
       <c r="E68" t="s">
-        <v>70</v>
+        <v>231</v>
       </c>
       <c r="F68" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="G68" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -5599,23 +5693,19 @@
         <v>64</v>
       </c>
       <c r="B69" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C69" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="D69" s="5">
-        <f>A68</f>
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="F69" t="s">
-        <v>8</v>
+        <v>216</v>
       </c>
       <c r="G69" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -5624,23 +5714,23 @@
         <v>65</v>
       </c>
       <c r="B70" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C70" s="14">
         <v>0.5</v>
       </c>
       <c r="D70" s="5">
-        <f t="shared" ref="D70:D73" si="6">A69</f>
+        <f>A69</f>
         <v>64</v>
       </c>
       <c r="E70" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F70" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G70" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -5649,20 +5739,20 @@
         <v>66</v>
       </c>
       <c r="B71" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C71" s="14">
         <v>0.5</v>
       </c>
       <c r="D71" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="D71:D74" si="6">A70</f>
         <v>65</v>
       </c>
       <c r="E71" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F71" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G71" t="s">
         <v>12</v>
@@ -5674,7 +5764,7 @@
         <v>67</v>
       </c>
       <c r="B72" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C72" s="14">
         <v>0.5</v>
@@ -5684,10 +5774,10 @@
         <v>66</v>
       </c>
       <c r="E72" t="s">
-        <v>200</v>
+        <v>13</v>
       </c>
       <c r="F72" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G72" t="s">
         <v>12</v>
@@ -5699,23 +5789,23 @@
         <v>68</v>
       </c>
       <c r="B73" t="s">
-        <v>57</v>
+        <v>133</v>
       </c>
       <c r="C73" s="14">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D73" s="5">
         <f t="shared" si="6"/>
         <v>67</v>
       </c>
       <c r="E73" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F73" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G73" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -5724,19 +5814,23 @@
         <v>69</v>
       </c>
       <c r="B74" t="s">
-        <v>134</v>
+        <v>57</v>
       </c>
       <c r="C74" s="14">
         <v>1</v>
       </c>
+      <c r="D74" s="5">
+        <f t="shared" si="6"/>
+        <v>68</v>
+      </c>
       <c r="E74" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="F74" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G74" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -5745,19 +5839,16 @@
         <v>70</v>
       </c>
       <c r="B75" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C75" s="14">
         <v>1</v>
       </c>
-      <c r="D75" s="5" t="s">
-        <v>263</v>
-      </c>
       <c r="E75" t="s">
-        <v>53</v>
+        <v>201</v>
       </c>
       <c r="F75" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G75" t="s">
         <v>6</v>
@@ -5769,48 +5860,47 @@
         <v>71</v>
       </c>
       <c r="B76" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C76" s="14">
         <v>1</v>
       </c>
-      <c r="D76" s="5">
-        <f>A75</f>
-        <v>70</v>
+      <c r="D76" s="5" t="s">
+        <v>263</v>
       </c>
       <c r="E76" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="F76" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G76" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77">
+      <c r="A77" s="8">
         <f t="shared" si="4"/>
         <v>72</v>
       </c>
       <c r="B77" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C77" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D77" s="5">
-        <f>A73</f>
-        <v>68</v>
+        <f>A76</f>
+        <v>71</v>
       </c>
       <c r="E77" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F77" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G77" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -5819,23 +5909,23 @@
         <v>73</v>
       </c>
       <c r="B78" t="s">
-        <v>170</v>
+        <v>137</v>
       </c>
       <c r="C78" s="14">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D78" s="5">
-        <f>A77</f>
-        <v>72</v>
+        <f>A74</f>
+        <v>69</v>
       </c>
       <c r="E78" t="s">
-        <v>204</v>
+        <v>23</v>
       </c>
       <c r="F78" t="s">
-        <v>218</v>
+        <v>24</v>
       </c>
       <c r="G78" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -5844,22 +5934,23 @@
         <v>74</v>
       </c>
       <c r="B79" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C79" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>264</v>
+        <v>1.5</v>
+      </c>
+      <c r="D79" s="5">
+        <f>A78</f>
+        <v>73</v>
       </c>
       <c r="E79" t="s">
-        <v>174</v>
+        <v>204</v>
       </c>
       <c r="F79" t="s">
-        <v>29</v>
+        <v>218</v>
       </c>
       <c r="G79" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -5867,24 +5958,23 @@
         <f t="shared" si="4"/>
         <v>75</v>
       </c>
-      <c r="B80" s="6" t="s">
-        <v>169</v>
+      <c r="B80" t="s">
+        <v>175</v>
       </c>
       <c r="C80" s="14">
-        <v>1</v>
-      </c>
-      <c r="D80" s="5">
-        <f>A77</f>
-        <v>72</v>
+        <v>0.5</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>264</v>
       </c>
       <c r="E80" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F80" t="s">
-        <v>220</v>
+        <v>29</v>
       </c>
       <c r="G80" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -5892,17 +5982,18 @@
         <f t="shared" si="4"/>
         <v>76</v>
       </c>
-      <c r="B81" t="s">
-        <v>171</v>
+      <c r="B81" s="6" t="s">
+        <v>169</v>
       </c>
       <c r="C81" s="14">
         <v>1</v>
       </c>
-      <c r="D81" s="5" t="s">
-        <v>265</v>
+      <c r="D81" s="5">
+        <f>A78</f>
+        <v>73</v>
       </c>
       <c r="E81" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F81" t="s">
         <v>220</v>
@@ -5917,17 +6008,16 @@
         <v>77</v>
       </c>
       <c r="B82" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C82" s="14">
         <v>1</v>
       </c>
-      <c r="D82" s="5">
-        <f>A81</f>
-        <v>76</v>
+      <c r="D82" s="5" t="s">
+        <v>265</v>
       </c>
       <c r="E82" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F82" t="s">
         <v>220</v>
@@ -5937,21 +6027,22 @@
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="8">
-        <f>ROW()-5</f>
+      <c r="A83">
+        <f t="shared" si="4"/>
         <v>78</v>
       </c>
       <c r="B83" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C83" s="14">
         <v>1</v>
       </c>
-      <c r="D83" s="5" t="s">
-        <v>267</v>
+      <c r="D83" s="5">
+        <f>A82</f>
+        <v>77</v>
       </c>
       <c r="E83" t="s">
-        <v>205</v>
+        <v>178</v>
       </c>
       <c r="F83" t="s">
         <v>220</v>
@@ -5961,72 +6052,72 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84">
+      <c r="A84" s="8">
+        <f>ROW()-5</f>
+        <v>79</v>
+      </c>
+      <c r="B84" t="s">
+        <v>173</v>
+      </c>
+      <c r="C84" s="14">
+        <v>1</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="E84" t="s">
+        <v>205</v>
+      </c>
+      <c r="F84" t="s">
+        <v>220</v>
+      </c>
+      <c r="G84" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85">
         <f t="shared" si="4"/>
-        <v>79</v>
-      </c>
-      <c r="B84" t="s">
+        <v>80</v>
+      </c>
+      <c r="B85" t="s">
         <v>180</v>
       </c>
-      <c r="C84" s="14">
+      <c r="C85" s="14">
         <v>2</v>
       </c>
-      <c r="D84" s="5" t="s">
+      <c r="D85" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E85" t="s">
         <v>110</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F85" t="s">
         <v>222</v>
       </c>
-      <c r="G84" t="s">
+      <c r="G85" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="8">
-        <f t="shared" ref="A85:A95" si="7">ROW()-5</f>
-        <v>80</v>
-      </c>
-      <c r="B85" t="s">
-        <v>117</v>
-      </c>
-      <c r="C85" s="14">
-        <v>3</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="E85" t="s">
-        <v>118</v>
-      </c>
-      <c r="F85" t="s">
-        <v>232</v>
-      </c>
-      <c r="G85" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="A86:A96" si="7">ROW()-5</f>
         <v>81</v>
       </c>
       <c r="B86" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C86" s="14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>277</v>
       </c>
       <c r="E86" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F86" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G86" t="s">
         <v>6</v>
@@ -6038,7 +6129,7 @@
         <v>82</v>
       </c>
       <c r="B87" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C87" s="14">
         <v>2</v>
@@ -6047,7 +6138,7 @@
         <v>277</v>
       </c>
       <c r="E87" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F87" t="s">
         <v>233</v>
@@ -6062,19 +6153,19 @@
         <v>83</v>
       </c>
       <c r="B88" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C88" s="14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D88" s="5" t="s">
         <v>277</v>
       </c>
       <c r="E88" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F88" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G88" t="s">
         <v>6</v>
@@ -6086,23 +6177,22 @@
         <v>84</v>
       </c>
       <c r="B89" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="C89" s="14">
-        <v>1</v>
-      </c>
-      <c r="D89" s="5">
-        <f>A23</f>
-        <v>20</v>
+        <v>4</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>277</v>
       </c>
       <c r="E89" t="s">
-        <v>94</v>
+        <v>124</v>
       </c>
       <c r="F89" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G89" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -6111,19 +6201,20 @@
         <v>85</v>
       </c>
       <c r="B90" t="s">
-        <v>184</v>
+        <v>107</v>
       </c>
       <c r="C90" s="14">
         <v>1</v>
       </c>
       <c r="D90" s="5">
-        <v>84</v>
+        <f>A23</f>
+        <v>20</v>
       </c>
       <c r="E90" t="s">
-        <v>237</v>
+        <v>94</v>
       </c>
       <c r="F90" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G90" t="s">
         <v>34</v>
@@ -6135,23 +6226,22 @@
         <v>86</v>
       </c>
       <c r="B91" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C91" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D91" s="5">
-        <f>A19</f>
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="E91" t="s">
-        <v>181</v>
+        <v>237</v>
       </c>
       <c r="F91" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G91" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -6160,20 +6250,20 @@
         <v>87</v>
       </c>
       <c r="B92" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C92" s="14">
         <v>2</v>
       </c>
       <c r="D92" s="5">
-        <f>A91</f>
-        <v>86</v>
+        <f>A19</f>
+        <v>16</v>
       </c>
       <c r="E92" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F92" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G92" t="s">
         <v>6</v>
@@ -6184,20 +6274,24 @@
         <f t="shared" si="7"/>
         <v>88</v>
       </c>
-      <c r="B93" s="6" t="s">
-        <v>240</v>
+      <c r="B93" t="s">
+        <v>179</v>
       </c>
       <c r="C93" s="14">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D93" s="5">
+        <f>A92</f>
+        <v>87</v>
       </c>
       <c r="E93" t="s">
-        <v>91</v>
+        <v>182</v>
       </c>
       <c r="F93" t="s">
-        <v>31</v>
+        <v>239</v>
       </c>
       <c r="G93" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -6205,23 +6299,20 @@
         <f t="shared" si="7"/>
         <v>89</v>
       </c>
-      <c r="B94" t="s">
-        <v>183</v>
+      <c r="B94" s="6" t="s">
+        <v>240</v>
       </c>
       <c r="C94" s="14">
-        <v>1.5</v>
-      </c>
-      <c r="D94" s="5" t="s">
-        <v>269</v>
+        <v>1</v>
       </c>
       <c r="E94" t="s">
-        <v>188</v>
+        <v>91</v>
       </c>
       <c r="F94" t="s">
-        <v>241</v>
+        <v>31</v>
       </c>
       <c r="G94" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -6230,43 +6321,46 @@
         <v>90</v>
       </c>
       <c r="B95" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C95" s="14">
         <v>1.5</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E95" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F95" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G95" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <f t="shared" si="4"/>
+      <c r="A96" s="8">
+        <f t="shared" si="7"/>
         <v>91</v>
       </c>
       <c r="B96" t="s">
-        <v>111</v>
+        <v>189</v>
       </c>
       <c r="C96" s="14">
-        <v>1</v>
+        <v>1.5</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>270</v>
       </c>
       <c r="E96" t="s">
-        <v>112</v>
+        <v>191</v>
       </c>
       <c r="F96" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G96" t="s">
-        <v>125</v>
+        <v>34</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -6275,23 +6369,19 @@
         <v>92</v>
       </c>
       <c r="B97" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C97" s="14">
-        <v>2</v>
-      </c>
-      <c r="D97" s="5">
-        <f>A96</f>
-        <v>91</v>
+        <v>1</v>
       </c>
       <c r="E97" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F97" t="s">
-        <v>22</v>
+        <v>243</v>
       </c>
       <c r="G97" t="s">
-        <v>6</v>
+        <v>125</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -6300,67 +6390,71 @@
         <v>93</v>
       </c>
       <c r="B98" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="C98" s="14">
-        <v>1</v>
-      </c>
-      <c r="D98" s="5" t="s">
-        <v>271</v>
+        <v>2</v>
+      </c>
+      <c r="D98" s="5">
+        <f>A97</f>
+        <v>92</v>
       </c>
       <c r="E98" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="F98" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="G98" t="s">
-        <v>125</v>
+        <v>6</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99">
-        <f t="shared" ref="A99:A108" si="8">ROW()-5</f>
+        <f t="shared" si="4"/>
         <v>94</v>
       </c>
       <c r="B99" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="C99" s="14">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>36</v>
+        <v>271</v>
       </c>
       <c r="E99" t="s">
-        <v>245</v>
+        <v>126</v>
       </c>
       <c r="F99" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G99" t="s">
-        <v>247</v>
+        <v>125</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="A100:A109" si="8">ROW()-5</f>
         <v>95</v>
       </c>
       <c r="B100" t="s">
-        <v>185</v>
+        <v>116</v>
       </c>
       <c r="C100" s="14">
-        <v>1</v>
+        <v>1.5</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="E100" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="F100" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G100" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -6369,40 +6463,40 @@
         <v>96</v>
       </c>
       <c r="B101" t="s">
+        <v>185</v>
+      </c>
+      <c r="C101" s="14">
+        <v>1</v>
+      </c>
+      <c r="E101" t="s">
+        <v>250</v>
+      </c>
+      <c r="F101" t="s">
+        <v>249</v>
+      </c>
+      <c r="G101" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <f t="shared" si="8"/>
+        <v>97</v>
+      </c>
+      <c r="B102" t="s">
         <v>186</v>
       </c>
-      <c r="C101" s="14">
-        <v>1</v>
-      </c>
-      <c r="D101" s="5" t="s">
+      <c r="C102" s="14">
+        <v>1</v>
+      </c>
+      <c r="D102" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E102" t="s">
         <v>187</v>
       </c>
-      <c r="F101" t="s">
+      <c r="F102" t="s">
         <v>222</v>
-      </c>
-      <c r="G101" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="8">
-        <f>ROW()-5</f>
-        <v>97</v>
-      </c>
-      <c r="B102" t="s">
-        <v>197</v>
-      </c>
-      <c r="C102" s="14">
-        <v>1</v>
-      </c>
-      <c r="E102" t="s">
-        <v>251</v>
-      </c>
-      <c r="F102" t="s">
-        <v>249</v>
       </c>
       <c r="G102" t="s">
         <v>76</v>
@@ -6414,43 +6508,43 @@
         <v>98</v>
       </c>
       <c r="B103" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C103" s="14">
         <v>1</v>
       </c>
-      <c r="D103" s="5" t="s">
-        <v>273</v>
-      </c>
       <c r="E103" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F103" t="s">
-        <v>222</v>
+        <v>249</v>
       </c>
       <c r="G103" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104">
-        <f t="shared" si="8"/>
+      <c r="A104" s="8">
+        <f>ROW()-5</f>
         <v>99</v>
       </c>
       <c r="B104" t="s">
-        <v>115</v>
+        <v>198</v>
       </c>
       <c r="C104" s="14">
         <v>1</v>
       </c>
-      <c r="E104" s="6" t="s">
-        <v>253</v>
+      <c r="D104" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="E104" t="s">
+        <v>252</v>
       </c>
       <c r="F104" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="G104" t="s">
-        <v>254</v>
+        <v>76</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -6459,22 +6553,19 @@
         <v>100</v>
       </c>
       <c r="B105" t="s">
-        <v>192</v>
+        <v>115</v>
       </c>
       <c r="C105" s="14">
-        <v>2</v>
-      </c>
-      <c r="D105" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="E105" t="s">
-        <v>255</v>
+        <v>1</v>
+      </c>
+      <c r="E105" s="6" t="s">
+        <v>253</v>
       </c>
       <c r="F105" t="s">
-        <v>256</v>
+        <v>217</v>
       </c>
       <c r="G105" t="s">
-        <v>6</v>
+        <v>254</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -6483,16 +6574,19 @@
         <v>101</v>
       </c>
       <c r="B106" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C106" s="14">
-        <v>1.5</v>
+        <v>2</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>274</v>
       </c>
       <c r="E106" t="s">
-        <v>193</v>
+        <v>255</v>
       </c>
       <c r="F106" t="s">
-        <v>190</v>
+        <v>256</v>
       </c>
       <c r="G106" t="s">
         <v>6</v>
@@ -6504,19 +6598,16 @@
         <v>102</v>
       </c>
       <c r="B107" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C107" s="14">
-        <v>1</v>
-      </c>
-      <c r="D107" s="5" t="s">
-        <v>275</v>
+        <v>1.5</v>
       </c>
       <c r="E107" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="F107" t="s">
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="G107" t="s">
         <v>6</v>
@@ -6528,16 +6619,16 @@
         <v>103</v>
       </c>
       <c r="B108" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C108" s="14">
         <v>1</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E108" t="s">
-        <v>257</v>
+        <v>205</v>
       </c>
       <c r="F108" t="s">
         <v>220</v>
@@ -6547,7 +6638,28 @@
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C109" s="14"/>
+      <c r="A109">
+        <f t="shared" si="8"/>
+        <v>104</v>
+      </c>
+      <c r="B109" t="s">
+        <v>196</v>
+      </c>
+      <c r="C109" s="14">
+        <v>1</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="E109" t="s">
+        <v>257</v>
+      </c>
+      <c r="F109" t="s">
+        <v>220</v>
+      </c>
+      <c r="G109" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C110" s="14"/>
@@ -6558,54 +6670,53 @@
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C112" s="14"/>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C113" s="14"/>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C114" s="14"/>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C115" s="14"/>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C116" s="14"/>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C117" s="14"/>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C118" s="14"/>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C119" s="14"/>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C120" s="14"/>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C121" s="14"/>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C122" s="14"/>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C123" s="14"/>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C124" s="14"/>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C125" s="14"/>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C126" s="14"/>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B127" s="6"/>
+    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C127" s="14"/>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="8"/>
+    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B128" s="6"/>
       <c r="C128" s="14"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -6638,7 +6749,6 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="8"/>
-      <c r="B136" s="6"/>
       <c r="C136" s="14"/>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -6648,20 +6758,25 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="8"/>
+      <c r="B138" s="6"/>
       <c r="C138" s="14"/>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="8"/>
       <c r="C139" s="14"/>
     </row>
-    <row r="160" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C160" s="2"/>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="8"/>
+      <c r="C140" s="14"/>
     </row>
     <row r="161" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C161" s="2"/>
     </row>
     <row r="162" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C162" s="2"/>
+    </row>
+    <row r="163" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C163" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6674,7 +6789,7 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="D17" twoDigitTextYear="1"/>
-    <ignoredError sqref="D77 D62" formula="1"/>
+    <ignoredError sqref="D78 D63" formula="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -6685,10 +6800,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54278537-4330-487B-8B1E-186EA2F14073}">
-  <dimension ref="A1:XFD121"/>
+  <dimension ref="A1:XFD122"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7362,8 +7477,8 @@
       <c r="I16" s="20"/>
       <c r="J16" s="20"/>
       <c r="K16" s="21"/>
-      <c r="L16" s="54"/>
-      <c r="M16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="54"/>
       <c r="N16" s="21"/>
       <c r="O16" s="21"/>
       <c r="P16" s="20"/>
@@ -8951,84 +9066,84 @@
       </c>
     </row>
     <row r="55" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A55" s="17">
+      <c r="A55" s="67">
         <f>Tâches!A53</f>
         <v>48</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="65" t="s">
+        <v>315</v>
+      </c>
+      <c r="C55" s="27" t="str">
+        <f>Tâches!B53</f>
+        <v>Gérer les UUID</v>
+      </c>
+      <c r="D55" s="68"/>
+      <c r="E55" s="69"/>
+      <c r="F55" s="69"/>
+      <c r="G55" s="69"/>
+      <c r="H55" s="69"/>
+      <c r="I55" s="70"/>
+      <c r="J55" s="71"/>
+      <c r="K55" s="69"/>
+      <c r="L55" s="69"/>
+      <c r="M55" s="69"/>
+      <c r="N55" s="69"/>
+      <c r="O55" s="69"/>
+      <c r="P55" s="70"/>
+      <c r="Q55" s="70"/>
+      <c r="R55" s="69"/>
+      <c r="S55" s="69"/>
+      <c r="T55" s="69"/>
+      <c r="U55" s="69"/>
+      <c r="V55" s="69"/>
+      <c r="W55" s="70"/>
+      <c r="X55" s="70"/>
+      <c r="Y55" s="69"/>
+      <c r="Z55" s="69"/>
+      <c r="AA55" s="69"/>
+      <c r="AB55" s="69"/>
+      <c r="AC55" s="69"/>
+      <c r="AD55" s="72"/>
+    </row>
+    <row r="56" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A56" s="17">
+        <f>Tâches!A53</f>
+        <v>48</v>
+      </c>
+      <c r="B56" t="s">
         <v>316</v>
       </c>
-      <c r="C55" s="17" t="str">
-        <f>Tâches!B53</f>
+      <c r="C56" s="17" t="str">
+        <f>Tâches!B54</f>
         <v>Analyser et explorer les données SIRENE de l'INSEE</v>
       </c>
-      <c r="D55" s="24"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="25"/>
-      <c r="H55" s="25"/>
-      <c r="I55" s="19"/>
-      <c r="J55" s="19"/>
-      <c r="K55" s="25"/>
-      <c r="L55" s="25"/>
-      <c r="M55" s="25"/>
-      <c r="N55" s="25"/>
-      <c r="O55" s="25"/>
-      <c r="P55" s="19"/>
-      <c r="Q55" s="19"/>
-      <c r="R55" s="25"/>
-      <c r="S55" s="25"/>
-      <c r="T55" s="25"/>
-      <c r="U55" s="25"/>
-      <c r="V55" s="25"/>
-      <c r="W55" s="19"/>
-      <c r="X55" s="19"/>
-      <c r="Y55" s="25"/>
-      <c r="Z55" s="25"/>
-      <c r="AA55" s="25"/>
-      <c r="AB55" s="25"/>
-      <c r="AC55" s="25"/>
-      <c r="AD55" s="26"/>
-    </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A56" s="18">
-        <f>Tâches!A54</f>
-        <v>49</v>
-      </c>
-      <c r="B56" t="s">
-        <v>314</v>
-      </c>
-      <c r="C56" s="18" t="str">
-        <f>Tâches!B54</f>
-        <v>Adapter le dictionnaire avec les données SIRENE de l'INSEE</v>
-      </c>
-      <c r="D56" s="22"/>
-      <c r="E56" s="21"/>
-      <c r="F56" s="21"/>
-      <c r="G56" s="21"/>
-      <c r="H56" s="21"/>
-      <c r="I56" s="20"/>
-      <c r="J56" s="20"/>
-      <c r="K56" s="21"/>
-      <c r="L56" s="21"/>
-      <c r="M56" s="21"/>
-      <c r="N56" s="21"/>
-      <c r="O56" s="21"/>
-      <c r="P56" s="20"/>
-      <c r="Q56" s="20"/>
-      <c r="R56" s="21"/>
-      <c r="S56" s="21"/>
-      <c r="T56" s="21"/>
-      <c r="U56" s="21"/>
-      <c r="V56" s="21"/>
-      <c r="W56" s="20"/>
-      <c r="X56" s="20"/>
-      <c r="Y56" s="21"/>
-      <c r="Z56" s="21"/>
-      <c r="AA56" s="21"/>
-      <c r="AB56" s="21"/>
-      <c r="AC56" s="21"/>
-      <c r="AD56" s="23"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="25"/>
+      <c r="F56" s="25"/>
+      <c r="G56" s="25"/>
+      <c r="H56" s="25"/>
+      <c r="I56" s="19"/>
+      <c r="J56" s="19"/>
+      <c r="K56" s="25"/>
+      <c r="L56" s="25"/>
+      <c r="M56" s="25"/>
+      <c r="N56" s="25"/>
+      <c r="O56" s="25"/>
+      <c r="P56" s="19"/>
+      <c r="Q56" s="19"/>
+      <c r="R56" s="25"/>
+      <c r="S56" s="25"/>
+      <c r="T56" s="25"/>
+      <c r="U56" s="25"/>
+      <c r="V56" s="25"/>
+      <c r="W56" s="19"/>
+      <c r="X56" s="19"/>
+      <c r="Y56" s="25"/>
+      <c r="Z56" s="25"/>
+      <c r="AA56" s="25"/>
+      <c r="AB56" s="25"/>
+      <c r="AC56" s="25"/>
+      <c r="AD56" s="26"/>
     </row>
     <row r="57" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A57" s="18">
@@ -9040,7 +9155,7 @@
       </c>
       <c r="C57" s="18" t="str">
         <f>Tâches!B55</f>
-        <v>Adapter le MCD avec les  données SIRENE de l'INSEE</v>
+        <v>Adapter le dictionnaire avec les données SIRENE de l'INSEE</v>
       </c>
       <c r="D57" s="22"/>
       <c r="E57" s="21"/>
@@ -9080,7 +9195,7 @@
       </c>
       <c r="C58" s="18" t="str">
         <f>Tâches!B56</f>
-        <v>Adapter le MLD avec les données SIRENE de l'INSEE</v>
+        <v>Adapter le MCD avec les  données SIRENE de l'INSEE</v>
       </c>
       <c r="D58" s="22"/>
       <c r="E58" s="21"/>
@@ -9120,7 +9235,7 @@
       </c>
       <c r="C59" s="18" t="str">
         <f>Tâches!B57</f>
-        <v>Adapter le MRD avec les données SIRENE de l'INSEE</v>
+        <v>Adapter le MLD avec les données SIRENE de l'INSEE</v>
       </c>
       <c r="D59" s="22"/>
       <c r="E59" s="21"/>
@@ -9156,11 +9271,11 @@
         <v>53</v>
       </c>
       <c r="B60" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C60" s="18" t="str">
         <f>Tâches!B58</f>
-        <v>Compléter la base de données avec les tables SIRENE pour l'INSEE</v>
+        <v>Adapter le MRD avec les données SIRENE de l'INSEE</v>
       </c>
       <c r="D60" s="22"/>
       <c r="E60" s="21"/>
@@ -9196,11 +9311,11 @@
         <v>54</v>
       </c>
       <c r="B61" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C61" s="18" t="str">
         <f>Tâches!B59</f>
-        <v>Détecter les anomalies et nettoyer les données SIRENE de l'INSEE</v>
+        <v>Compléter la base de données avec les tables SIRENE pour l'INSEE</v>
       </c>
       <c r="D61" s="22"/>
       <c r="E61" s="21"/>
@@ -9240,7 +9355,7 @@
       </c>
       <c r="C62" s="18" t="str">
         <f>Tâches!B60</f>
-        <v>Mettre en forme les données SIRENE de l'INSEE</v>
+        <v>Détecter les anomalies et nettoyer les données SIRENE de l'INSEE</v>
       </c>
       <c r="D62" s="22"/>
       <c r="E62" s="21"/>
@@ -9280,7 +9395,7 @@
       </c>
       <c r="C63" s="18" t="str">
         <f>Tâches!B61</f>
-        <v>Intégrer dans la base de données les données SIRENE de l'INSEE</v>
+        <v>Mettre en forme les données SIRENE de l'INSEE</v>
       </c>
       <c r="D63" s="22"/>
       <c r="E63" s="21"/>
@@ -9316,11 +9431,11 @@
         <v>57</v>
       </c>
       <c r="B64" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C64" s="18" t="str">
         <f>Tâches!B62</f>
-        <v>Créer des requêtes (CRUD) pour les données SIRENE de l'INSEE</v>
+        <v>Intégrer dans la base de données les données SIRENE de l'INSEE</v>
       </c>
       <c r="D64" s="22"/>
       <c r="E64" s="21"/>
@@ -9356,11 +9471,11 @@
         <v>58</v>
       </c>
       <c r="B65" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C65" s="18" t="str">
         <f>Tâches!B63</f>
-        <v>Créer les graphiques en croisant les données actuelles et celles SIRENE de l'INSEE</v>
+        <v>Créer des requêtes (CRUD) pour les données SIRENE de l'INSEE</v>
       </c>
       <c r="D65" s="22"/>
       <c r="E65" s="21"/>
@@ -9396,11 +9511,11 @@
         <v>59</v>
       </c>
       <c r="B66" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C66" s="18" t="str">
         <f>Tâches!B64</f>
-        <v>Intégrer les nouveaux graphiques croisés CACPL/INSEE dans le tableau de bord</v>
+        <v>Créer les graphiques en croisant les données actuelles et celles SIRENE de l'INSEE</v>
       </c>
       <c r="D66" s="22"/>
       <c r="E66" s="21"/>
@@ -9436,11 +9551,11 @@
         <v>60</v>
       </c>
       <c r="B67" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C67" s="18" t="str">
         <f>Tâches!B65</f>
-        <v>Afficher sur la carte les sociétés</v>
+        <v>Intégrer les nouveaux graphiques croisés CACPL/INSEE dans le tableau de bord</v>
       </c>
       <c r="D67" s="22"/>
       <c r="E67" s="21"/>
@@ -9480,7 +9595,7 @@
       </c>
       <c r="C68" s="18" t="str">
         <f>Tâches!B66</f>
-        <v>Afficher sur la carte les filtres issus des données SIRENE de l'INSEE</v>
+        <v>Afficher sur la carte les sociétés</v>
       </c>
       <c r="D68" s="22"/>
       <c r="E68" s="21"/>
@@ -9516,11 +9631,11 @@
         <v>62</v>
       </c>
       <c r="B69" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C69" s="18" t="str">
         <f>Tâches!B67</f>
-        <v>Interpréter l'adéquation entre collecteurs et chiffres SIRENE de l'INSEE</v>
+        <v>Afficher sur la carte les filtres issus des données SIRENE de l'INSEE</v>
       </c>
       <c r="D69" s="22"/>
       <c r="E69" s="21"/>
@@ -9556,11 +9671,11 @@
         <v>63</v>
       </c>
       <c r="B70" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C70" s="18" t="str">
         <f>Tâches!B68</f>
-        <v>Analyser et explorer les nouvelles données de la CACPL</v>
+        <v>Interpréter l'adéquation entre collecteurs et chiffres SIRENE de l'INSEE</v>
       </c>
       <c r="D70" s="22"/>
       <c r="E70" s="21"/>
@@ -9596,11 +9711,11 @@
         <v>64</v>
       </c>
       <c r="B71" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C71" s="18" t="str">
         <f>Tâches!B69</f>
-        <v>Adapter le dictionnaire aux nouvelles données de la CACPL</v>
+        <v>Analyser et explorer les nouvelles données de la CACPL</v>
       </c>
       <c r="D71" s="22"/>
       <c r="E71" s="21"/>
@@ -9640,7 +9755,7 @@
       </c>
       <c r="C72" s="18" t="str">
         <f>Tâches!B70</f>
-        <v>Adapter le MCD avec les nouvelles données de la CACPL</v>
+        <v>Adapter le dictionnaire aux nouvelles données de la CACPL</v>
       </c>
       <c r="D72" s="22"/>
       <c r="E72" s="21"/>
@@ -9680,7 +9795,7 @@
       </c>
       <c r="C73" s="18" t="str">
         <f>Tâches!B71</f>
-        <v>Adapter le MLD avec les nouvelles données de la CACPL</v>
+        <v>Adapter le MCD avec les nouvelles données de la CACPL</v>
       </c>
       <c r="D73" s="22"/>
       <c r="E73" s="21"/>
@@ -9720,7 +9835,7 @@
       </c>
       <c r="C74" s="18" t="str">
         <f>Tâches!B72</f>
-        <v>Adapter le MRD avec les données de l'INSEE</v>
+        <v>Adapter le MLD avec les nouvelles données de la CACPL</v>
       </c>
       <c r="D74" s="22"/>
       <c r="E74" s="21"/>
@@ -9756,11 +9871,11 @@
         <v>68</v>
       </c>
       <c r="B75" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C75" s="18" t="str">
         <f>Tâches!B73</f>
-        <v>Compléter la base de données avec les tables pour l'INSEE</v>
+        <v>Adapter le MRD avec les données de l'INSEE</v>
       </c>
       <c r="D75" s="22"/>
       <c r="E75" s="21"/>
@@ -9796,11 +9911,11 @@
         <v>69</v>
       </c>
       <c r="B76" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C76" s="18" t="str">
         <f>Tâches!B74</f>
-        <v>Détecter les anomalies et nettoyer les nouvelles données de la CACPL</v>
+        <v>Compléter la base de données avec les tables pour l'INSEE</v>
       </c>
       <c r="D76" s="22"/>
       <c r="E76" s="21"/>
@@ -9840,7 +9955,7 @@
       </c>
       <c r="C77" s="18" t="str">
         <f>Tâches!B75</f>
-        <v>Mettre en forme les nouvelles données de la CACPL</v>
+        <v>Détecter les anomalies et nettoyer les nouvelles données de la CACPL</v>
       </c>
       <c r="D77" s="22"/>
       <c r="E77" s="21"/>
@@ -9880,7 +9995,7 @@
       </c>
       <c r="C78" s="18" t="str">
         <f>Tâches!B76</f>
-        <v>Intégrer dans la base de données les nouvelles données de la CACPL</v>
+        <v>Mettre en forme les nouvelles données de la CACPL</v>
       </c>
       <c r="D78" s="22"/>
       <c r="E78" s="21"/>
@@ -9916,11 +10031,11 @@
         <v>72</v>
       </c>
       <c r="B79" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C79" s="18" t="str">
         <f>Tâches!B77</f>
-        <v>Créer des requêtes (CRUD) pour les nouvelles données de la CACPL</v>
+        <v>Intégrer dans la base de données les nouvelles données de la CACPL</v>
       </c>
       <c r="D79" s="22"/>
       <c r="E79" s="21"/>
@@ -9956,11 +10071,11 @@
         <v>73</v>
       </c>
       <c r="B80" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C80" s="18" t="str">
         <f>Tâches!B78</f>
-        <v>Créer les graphiques croisant les données actuelles et les nouvelles de la CACPL</v>
+        <v>Créer des requêtes (CRUD) pour les nouvelles données de la CACPL</v>
       </c>
       <c r="D80" s="22"/>
       <c r="E80" s="21"/>
@@ -9996,11 +10111,11 @@
         <v>74</v>
       </c>
       <c r="B81" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C81" s="18" t="str">
         <f>Tâches!B79</f>
-        <v>Intégrer les nouveaux graphiques croisés de la CACPL dans le tableau de bord</v>
+        <v>Créer les graphiques croisant les données actuelles et les nouvelles de la CACPL</v>
       </c>
       <c r="D81" s="22"/>
       <c r="E81" s="21"/>
@@ -10036,11 +10151,11 @@
         <v>75</v>
       </c>
       <c r="B82" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C82" s="18" t="str">
         <f>Tâches!B80</f>
-        <v>Générer les nouveaux graphiques pour chaque déchèterie et chaque collecteur</v>
+        <v>Intégrer les nouveaux graphiques croisés de la CACPL dans le tableau de bord</v>
       </c>
       <c r="D82" s="22"/>
       <c r="E82" s="21"/>
@@ -10080,7 +10195,7 @@
       </c>
       <c r="C83" s="18" t="str">
         <f>Tâches!B81</f>
-        <v>Intégrer les graphiques pour chaque repère de la carte</v>
+        <v>Générer les nouveaux graphiques pour chaque déchèterie et chaque collecteur</v>
       </c>
       <c r="D83" s="22"/>
       <c r="E83" s="21"/>
@@ -10120,7 +10235,7 @@
       </c>
       <c r="C84" s="18" t="str">
         <f>Tâches!B82</f>
-        <v>Rendre dynamique les graphiques de chaque repère</v>
+        <v>Intégrer les graphiques pour chaque repère de la carte</v>
       </c>
       <c r="D84" s="22"/>
       <c r="E84" s="21"/>
@@ -10160,7 +10275,7 @@
       </c>
       <c r="C85" s="18" t="str">
         <f>Tâches!B83</f>
-        <v>Afficher sur la carte les filtres issus des nouvelles données de la CACPL</v>
+        <v>Rendre dynamique les graphiques de chaque repère</v>
       </c>
       <c r="D85" s="22"/>
       <c r="E85" s="21"/>
@@ -10196,11 +10311,11 @@
         <v>79</v>
       </c>
       <c r="B86" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C86" s="18" t="str">
         <f>Tâches!B84</f>
-        <v>Interpréter l'adéquation entre collecteurs et nouvelles données de la CACPL</v>
+        <v>Afficher sur la carte les filtres issus des nouvelles données de la CACPL</v>
       </c>
       <c r="D86" s="22"/>
       <c r="E86" s="21"/>
@@ -10236,11 +10351,11 @@
         <v>80</v>
       </c>
       <c r="B87" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C87" s="18" t="str">
         <f>Tâches!B85</f>
-        <v>Définir les facteurs principaux d'utilsation des collecteurs</v>
+        <v>Interpréter l'adéquation entre collecteurs et nouvelles données de la CACPL</v>
       </c>
       <c r="D87" s="22"/>
       <c r="E87" s="21"/>
@@ -10280,7 +10395,7 @@
       </c>
       <c r="C88" s="18" t="str">
         <f>Tâches!B86</f>
-        <v>Définir les types d'usager</v>
+        <v>Définir les facteurs principaux d'utilsation des collecteurs</v>
       </c>
       <c r="D88" s="22"/>
       <c r="E88" s="21"/>
@@ -10320,7 +10435,7 @@
       </c>
       <c r="C89" s="18" t="str">
         <f>Tâches!B87</f>
-        <v>Définir les groupes de collecteurs</v>
+        <v>Définir les types d'usager</v>
       </c>
       <c r="D89" s="22"/>
       <c r="E89" s="21"/>
@@ -10360,7 +10475,7 @@
       </c>
       <c r="C90" s="18" t="str">
         <f>Tâches!B88</f>
-        <v>Détecter et prévoir l'utilisation des collecteurs</v>
+        <v>Définir les groupes de collecteurs</v>
       </c>
       <c r="D90" s="22"/>
       <c r="E90" s="21"/>
@@ -10400,7 +10515,7 @@
       </c>
       <c r="C91" s="18" t="str">
         <f>Tâches!B89</f>
-        <v>Transformer le tableau de bord en service</v>
+        <v>Détecter et prévoir l'utilisation des collecteurs</v>
       </c>
       <c r="D91" s="22"/>
       <c r="E91" s="21"/>
@@ -10440,7 +10555,7 @@
       </c>
       <c r="C92" s="18" t="str">
         <f>Tâches!B90</f>
-        <v>Créer une API pour le service</v>
+        <v>Transformer le tableau de bord en service</v>
       </c>
       <c r="D92" s="22"/>
       <c r="E92" s="21"/>
@@ -10480,7 +10595,7 @@
       </c>
       <c r="C93" s="18" t="str">
         <f>Tâches!B91</f>
-        <v>Afficher et rendre éditable les tables de la BDD sur le tableau de bord</v>
+        <v>Créer une API pour le service</v>
       </c>
       <c r="D93" s="22"/>
       <c r="E93" s="21"/>
@@ -10520,7 +10635,7 @@
       </c>
       <c r="C94" s="18" t="str">
         <f>Tâches!B92</f>
-        <v xml:space="preserve">Gérer la persistance des données éditées dans la BDD </v>
+        <v>Afficher et rendre éditable les tables de la BDD sur le tableau de bord</v>
       </c>
       <c r="D94" s="22"/>
       <c r="E94" s="21"/>
@@ -10556,11 +10671,11 @@
         <v>88</v>
       </c>
       <c r="B95" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C95" s="18" t="str">
         <f>Tâches!B93</f>
-        <v>Créer le formulaire pour les comptes utilisateurs</v>
+        <v xml:space="preserve">Gérer la persistance des données éditées dans la BDD </v>
       </c>
       <c r="D95" s="22"/>
       <c r="E95" s="21"/>
@@ -10596,11 +10711,11 @@
         <v>89</v>
       </c>
       <c r="B96" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C96" s="18" t="str">
         <f>Tâches!B94</f>
-        <v xml:space="preserve">Gérer les comptes utilisateurs </v>
+        <v>Créer le formulaire pour les comptes utilisateurs</v>
       </c>
       <c r="D96" s="22"/>
       <c r="E96" s="21"/>
@@ -10640,7 +10755,7 @@
       </c>
       <c r="C97" s="18" t="str">
         <f>Tâches!B95</f>
-        <v>Restreindre l'accès de certaines fonctionnalités aux utilisateurs</v>
+        <v xml:space="preserve">Gérer les comptes utilisateurs </v>
       </c>
       <c r="D97" s="22"/>
       <c r="E97" s="21"/>
@@ -10676,11 +10791,11 @@
         <v>91</v>
       </c>
       <c r="B98" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C98" s="18" t="str">
         <f>Tâches!B96</f>
-        <v>Créer un data lake pour tous les jeux de données</v>
+        <v>Restreindre l'accès de certaines fonctionnalités aux utilisateurs</v>
       </c>
       <c r="D98" s="22"/>
       <c r="E98" s="21"/>
@@ -10720,7 +10835,7 @@
       </c>
       <c r="C99" s="18" t="str">
         <f>Tâches!B97</f>
-        <v>Intégrer les jeux de données dans le data lake</v>
+        <v>Créer un data lake pour tous les jeux de données</v>
       </c>
       <c r="D99" s="22"/>
       <c r="E99" s="21"/>
@@ -10756,11 +10871,11 @@
         <v>93</v>
       </c>
       <c r="B100" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C100" s="18" t="str">
         <f>Tâches!B98</f>
-        <v>Récupérer et éditer les informations du data lake</v>
+        <v>Intégrer les jeux de données dans le data lake</v>
       </c>
       <c r="D100" s="22"/>
       <c r="E100" s="21"/>
@@ -10796,11 +10911,11 @@
         <v>94</v>
       </c>
       <c r="B101" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C101" s="18" t="str">
         <f>Tâches!B99</f>
-        <v>Créer un exécutable</v>
+        <v>Récupérer et éditer les informations du data lake</v>
       </c>
       <c r="D101" s="22"/>
       <c r="E101" s="21"/>
@@ -10831,38 +10946,38 @@
       <c r="AD101" s="23"/>
     </row>
     <row r="102" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A102" s="27">
+      <c r="A102" s="18">
         <f>Tâches!A100</f>
         <v>95</v>
       </c>
       <c r="B102" t="s">
-        <v>320</v>
-      </c>
-      <c r="C102" s="27" t="str">
+        <v>313</v>
+      </c>
+      <c r="C102" s="18" t="str">
         <f>Tâches!B100</f>
-        <v>Se documenter sur les directives quant à la gestion des déchets</v>
+        <v>Créer un exécutable</v>
       </c>
       <c r="D102" s="22"/>
       <c r="E102" s="21"/>
       <c r="F102" s="21"/>
       <c r="G102" s="21"/>
       <c r="H102" s="21"/>
-      <c r="I102" s="28"/>
-      <c r="J102" s="29"/>
+      <c r="I102" s="20"/>
+      <c r="J102" s="20"/>
       <c r="K102" s="21"/>
       <c r="L102" s="21"/>
       <c r="M102" s="21"/>
       <c r="N102" s="21"/>
       <c r="O102" s="21"/>
-      <c r="P102" s="28"/>
-      <c r="Q102" s="28"/>
+      <c r="P102" s="20"/>
+      <c r="Q102" s="20"/>
       <c r="R102" s="21"/>
       <c r="S102" s="21"/>
       <c r="T102" s="21"/>
       <c r="U102" s="21"/>
       <c r="V102" s="21"/>
-      <c r="W102" s="28"/>
-      <c r="X102" s="28"/>
+      <c r="W102" s="20"/>
+      <c r="X102" s="20"/>
       <c r="Y102" s="21"/>
       <c r="Z102" s="21"/>
       <c r="AA102" s="21"/>
@@ -10876,11 +10991,11 @@
         <v>96</v>
       </c>
       <c r="B103" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C103" s="27" t="str">
         <f>Tâches!B101</f>
-        <v>Evaluer la conformité de la CACPL vis-à-vis des directives sur les déchets</v>
+        <v>Se documenter sur les directives quant à la gestion des déchets</v>
       </c>
       <c r="D103" s="22"/>
       <c r="E103" s="21"/>
@@ -10916,11 +11031,11 @@
         <v>97</v>
       </c>
       <c r="B104" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C104" s="27" t="str">
         <f>Tâches!B102</f>
-        <v>Collecter les données et résultats de collecte d'autres villes</v>
+        <v>Evaluer la conformité de la CACPL vis-à-vis des directives sur les déchets</v>
       </c>
       <c r="D104" s="22"/>
       <c r="E104" s="21"/>
@@ -10956,11 +11071,11 @@
         <v>98</v>
       </c>
       <c r="B105" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C105" s="27" t="str">
         <f>Tâches!B103</f>
-        <v>Comparer les dispositifs de collecte et résultats de la CACPL avec ceux d'autres villes</v>
+        <v>Collecter les données et résultats de collecte d'autres villes</v>
       </c>
       <c r="D105" s="22"/>
       <c r="E105" s="21"/>
@@ -10996,11 +11111,11 @@
         <v>99</v>
       </c>
       <c r="B106" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C106" s="27" t="str">
         <f>Tâches!B104</f>
-        <v>Récupérer les données pertinentes sur le site de Météo-France</v>
+        <v>Comparer les dispositifs de collecte et résultats de la CACPL avec ceux d'autres villes</v>
       </c>
       <c r="D106" s="22"/>
       <c r="E106" s="21"/>
@@ -11036,11 +11151,11 @@
         <v>100</v>
       </c>
       <c r="B107" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="C107" s="27" t="str">
         <f>Tâches!B105</f>
-        <v>Détecter et prévoir l'utilisation des collecteurs selon la météo</v>
+        <v>Récupérer les données pertinentes sur le site de Météo-France</v>
       </c>
       <c r="D107" s="22"/>
       <c r="E107" s="21"/>
@@ -11080,7 +11195,7 @@
       </c>
       <c r="C108" s="27" t="str">
         <f>Tâches!B106</f>
-        <v>Récupérer les information météorologiques en continu</v>
+        <v>Détecter et prévoir l'utilisation des collecteurs selon la météo</v>
       </c>
       <c r="D108" s="22"/>
       <c r="E108" s="21"/>
@@ -11120,7 +11235,7 @@
       </c>
       <c r="C109" s="27" t="str">
         <f>Tâches!B107</f>
-        <v>Afficher sur la carte les filtres météo</v>
+        <v>Récupérer les information météorologiques en continu</v>
       </c>
       <c r="D109" s="22"/>
       <c r="E109" s="21"/>
@@ -11151,47 +11266,87 @@
       <c r="AD109" s="23"/>
     </row>
     <row r="110" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A110" s="36">
+      <c r="A110" s="27">
         <f>Tâches!A108</f>
         <v>103</v>
       </c>
-      <c r="B110" s="30" t="s">
+      <c r="B110" t="s">
         <v>316</v>
       </c>
-      <c r="C110" s="36" t="str">
+      <c r="C110" s="27" t="str">
         <f>Tâches!B108</f>
+        <v>Afficher sur la carte les filtres météo</v>
+      </c>
+      <c r="D110" s="22"/>
+      <c r="E110" s="21"/>
+      <c r="F110" s="21"/>
+      <c r="G110" s="21"/>
+      <c r="H110" s="21"/>
+      <c r="I110" s="28"/>
+      <c r="J110" s="29"/>
+      <c r="K110" s="21"/>
+      <c r="L110" s="21"/>
+      <c r="M110" s="21"/>
+      <c r="N110" s="21"/>
+      <c r="O110" s="21"/>
+      <c r="P110" s="28"/>
+      <c r="Q110" s="28"/>
+      <c r="R110" s="21"/>
+      <c r="S110" s="21"/>
+      <c r="T110" s="21"/>
+      <c r="U110" s="21"/>
+      <c r="V110" s="21"/>
+      <c r="W110" s="28"/>
+      <c r="X110" s="28"/>
+      <c r="Y110" s="21"/>
+      <c r="Z110" s="21"/>
+      <c r="AA110" s="21"/>
+      <c r="AB110" s="21"/>
+      <c r="AC110" s="21"/>
+      <c r="AD110" s="23"/>
+    </row>
+    <row r="111" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A111" s="36">
+        <f>Tâches!A109</f>
+        <v>104</v>
+      </c>
+      <c r="B111" s="30" t="s">
+        <v>316</v>
+      </c>
+      <c r="C111" s="36" t="str">
+        <f>Tâches!B109</f>
         <v>Actualiser les prévisions de collecte sur la carte selon la météo</v>
       </c>
-      <c r="D110" s="32"/>
-      <c r="E110" s="33"/>
-      <c r="F110" s="33"/>
-      <c r="G110" s="33"/>
-      <c r="H110" s="33"/>
-      <c r="I110" s="34"/>
-      <c r="J110" s="37"/>
-      <c r="K110" s="33"/>
-      <c r="L110" s="33"/>
-      <c r="M110" s="33"/>
-      <c r="N110" s="33"/>
-      <c r="O110" s="33"/>
-      <c r="P110" s="34"/>
-      <c r="Q110" s="34"/>
-      <c r="R110" s="33"/>
-      <c r="S110" s="33"/>
-      <c r="T110" s="33"/>
-      <c r="U110" s="33"/>
-      <c r="V110" s="33"/>
-      <c r="W110" s="34"/>
-      <c r="X110" s="34"/>
-      <c r="Y110" s="33"/>
-      <c r="Z110" s="33"/>
-      <c r="AA110" s="33"/>
-      <c r="AB110" s="33"/>
-      <c r="AC110" s="33"/>
-      <c r="AD110" s="35"/>
-    </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B121" s="16"/>
+      <c r="D111" s="32"/>
+      <c r="E111" s="33"/>
+      <c r="F111" s="33"/>
+      <c r="G111" s="33"/>
+      <c r="H111" s="33"/>
+      <c r="I111" s="34"/>
+      <c r="J111" s="37"/>
+      <c r="K111" s="33"/>
+      <c r="L111" s="33"/>
+      <c r="M111" s="33"/>
+      <c r="N111" s="33"/>
+      <c r="O111" s="33"/>
+      <c r="P111" s="34"/>
+      <c r="Q111" s="34"/>
+      <c r="R111" s="33"/>
+      <c r="S111" s="33"/>
+      <c r="T111" s="33"/>
+      <c r="U111" s="33"/>
+      <c r="V111" s="33"/>
+      <c r="W111" s="34"/>
+      <c r="X111" s="34"/>
+      <c r="Y111" s="33"/>
+      <c r="Z111" s="33"/>
+      <c r="AA111" s="33"/>
+      <c r="AB111" s="33"/>
+      <c r="AC111" s="33"/>
+      <c r="AD111" s="35"/>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B122" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -11209,7 +11364,7 @@
     <mergeCell ref="R3:X3"/>
     <mergeCell ref="Y3:AD3"/>
   </mergeCells>
-  <conditionalFormatting sqref="B5:B51 B55:B110">
+  <conditionalFormatting sqref="B5:B51 B55:B111">
     <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"Programmation"</formula>
     </cfRule>
@@ -11255,10 +11410,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H114"/>
+  <dimension ref="A1:H115"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11635,7 +11790,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="14">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="53">
@@ -11644,7 +11799,7 @@
       </c>
       <c r="G15" s="14">
         <f>IF(AvancementPrincipal[[#This Row],[Temps consacré (jours-hommes)]]&lt;&gt;"",AvancementPrincipal[[#This Row],[Durée estimée (jours-hommes)]]-AvancementPrincipal[[#This Row],[Temps consacré (jours-hommes)]]-AvancementPrincipal[[#This Row],[Temps restant (jours-hommes)]],"")</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H15" s="1"/>
     </row>
@@ -11662,7 +11817,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="14">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="53">
@@ -11671,7 +11826,7 @@
       </c>
       <c r="G16" s="14">
         <f>IF(AvancementPrincipal[[#This Row],[Temps consacré (jours-hommes)]]&lt;&gt;"",AvancementPrincipal[[#This Row],[Durée estimée (jours-hommes)]]-AvancementPrincipal[[#This Row],[Temps consacré (jours-hommes)]]-AvancementPrincipal[[#This Row],[Temps restant (jours-hommes)]],"")</f>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="H16" s="1"/>
     </row>
@@ -11688,15 +11843,17 @@
         <f>TachesPrincipales[[#This Row],[Travail (en jours-hommes)]]</f>
         <v>1</v>
       </c>
-      <c r="D17" s="14"/>
+      <c r="D17" s="14">
+        <v>0.5</v>
+      </c>
       <c r="E17" s="2"/>
       <c r="F17" s="53">
         <f>IFERROR(AvancementPrincipal[[#This Row],[Temps consacré (jours-hommes)]]/(AvancementPrincipal[[#This Row],[Temps consacré (jours-hommes)]]+AvancementPrincipal[[#This Row],[Temps restant (jours-hommes)]]), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G17" s="14" t="str">
+        <v>1</v>
+      </c>
+      <c r="G17" s="14">
         <f>IF(AvancementPrincipal[[#This Row],[Temps consacré (jours-hommes)]]&lt;&gt;"",AvancementPrincipal[[#This Row],[Durée estimée (jours-hommes)]]-AvancementPrincipal[[#This Row],[Temps consacré (jours-hommes)]]-AvancementPrincipal[[#This Row],[Temps restant (jours-hommes)]],"")</f>
-        <v/>
+        <v>0.5</v>
       </c>
       <c r="H17" s="1"/>
     </row>
@@ -11713,15 +11870,17 @@
         <f>TachesPrincipales[[#This Row],[Travail (en jours-hommes)]]</f>
         <v>1</v>
       </c>
-      <c r="D18" s="14"/>
+      <c r="D18" s="14">
+        <v>0.5</v>
+      </c>
       <c r="E18" s="2"/>
       <c r="F18" s="53">
         <f>IFERROR(AvancementPrincipal[[#This Row],[Temps consacré (jours-hommes)]]/(AvancementPrincipal[[#This Row],[Temps consacré (jours-hommes)]]+AvancementPrincipal[[#This Row],[Temps restant (jours-hommes)]]), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G18" s="14" t="str">
+        <v>1</v>
+      </c>
+      <c r="G18" s="14">
         <f>IF(AvancementPrincipal[[#This Row],[Temps consacré (jours-hommes)]]&lt;&gt;"",AvancementPrincipal[[#This Row],[Durée estimée (jours-hommes)]]-AvancementPrincipal[[#This Row],[Temps consacré (jours-hommes)]]-AvancementPrincipal[[#This Row],[Temps restant (jours-hommes)]],"")</f>
-        <v/>
+        <v>0.5</v>
       </c>
       <c r="H18" s="1"/>
     </row>
@@ -12574,11 +12733,11 @@
       </c>
       <c r="B53" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Analyser et explorer les données SIRENE de l'INSEE</v>
+        <v>Gérer les UUID</v>
       </c>
       <c r="C53" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D53" s="14"/>
       <c r="E53" s="14"/>
@@ -12593,17 +12752,17 @@
       <c r="H53" s="1"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="A54" s="8">
         <f>TachesBonus[[#This Row],[N°]]</f>
         <v>49</v>
       </c>
-      <c r="B54" t="str">
+      <c r="B54" s="8" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Adapter le dictionnaire avec les données SIRENE de l'INSEE</v>
+        <v>Analyser et explorer les données SIRENE de l'INSEE</v>
       </c>
       <c r="C54" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D54" s="14"/>
       <c r="E54" s="14"/>
@@ -12624,7 +12783,7 @@
       </c>
       <c r="B55" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Adapter le MCD avec les  données SIRENE de l'INSEE</v>
+        <v>Adapter le dictionnaire avec les données SIRENE de l'INSEE</v>
       </c>
       <c r="C55" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -12649,7 +12808,7 @@
       </c>
       <c r="B56" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Adapter le MLD avec les données SIRENE de l'INSEE</v>
+        <v>Adapter le MCD avec les  données SIRENE de l'INSEE</v>
       </c>
       <c r="C56" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -12674,7 +12833,7 @@
       </c>
       <c r="B57" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Adapter le MRD avec les données SIRENE de l'INSEE</v>
+        <v>Adapter le MLD avec les données SIRENE de l'INSEE</v>
       </c>
       <c r="C57" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -12699,11 +12858,11 @@
       </c>
       <c r="B58" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Compléter la base de données avec les tables SIRENE pour l'INSEE</v>
+        <v>Adapter le MRD avec les données SIRENE de l'INSEE</v>
       </c>
       <c r="C58" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D58" s="14"/>
       <c r="E58" s="14"/>
@@ -12724,7 +12883,7 @@
       </c>
       <c r="B59" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Détecter les anomalies et nettoyer les données SIRENE de l'INSEE</v>
+        <v>Compléter la base de données avec les tables SIRENE pour l'INSEE</v>
       </c>
       <c r="C59" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -12749,7 +12908,7 @@
       </c>
       <c r="B60" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Mettre en forme les données SIRENE de l'INSEE</v>
+        <v>Détecter les anomalies et nettoyer les données SIRENE de l'INSEE</v>
       </c>
       <c r="C60" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -12774,7 +12933,7 @@
       </c>
       <c r="B61" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Intégrer dans la base de données les données SIRENE de l'INSEE</v>
+        <v>Mettre en forme les données SIRENE de l'INSEE</v>
       </c>
       <c r="C61" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -12799,7 +12958,7 @@
       </c>
       <c r="B62" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Créer des requêtes (CRUD) pour les données SIRENE de l'INSEE</v>
+        <v>Intégrer dans la base de données les données SIRENE de l'INSEE</v>
       </c>
       <c r="C62" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -12824,7 +12983,7 @@
       </c>
       <c r="B63" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Créer les graphiques en croisant les données actuelles et celles SIRENE de l'INSEE</v>
+        <v>Créer des requêtes (CRUD) pour les données SIRENE de l'INSEE</v>
       </c>
       <c r="C63" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -12849,11 +13008,11 @@
       </c>
       <c r="B64" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Intégrer les nouveaux graphiques croisés CACPL/INSEE dans le tableau de bord</v>
+        <v>Créer les graphiques en croisant les données actuelles et celles SIRENE de l'INSEE</v>
       </c>
       <c r="C64" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D64" s="14"/>
       <c r="E64" s="14"/>
@@ -12874,11 +13033,11 @@
       </c>
       <c r="B65" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Afficher sur la carte les sociétés</v>
+        <v>Intégrer les nouveaux graphiques croisés CACPL/INSEE dans le tableau de bord</v>
       </c>
       <c r="C65" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D65" s="14"/>
       <c r="E65" s="14"/>
@@ -12899,7 +13058,7 @@
       </c>
       <c r="B66" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Afficher sur la carte les filtres issus des données SIRENE de l'INSEE</v>
+        <v>Afficher sur la carte les sociétés</v>
       </c>
       <c r="C66" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -12924,11 +13083,11 @@
       </c>
       <c r="B67" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Interpréter l'adéquation entre collecteurs et chiffres SIRENE de l'INSEE</v>
+        <v>Afficher sur la carte les filtres issus des données SIRENE de l'INSEE</v>
       </c>
       <c r="C67" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D67" s="14"/>
       <c r="E67" s="14"/>
@@ -12949,11 +13108,11 @@
       </c>
       <c r="B68" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Analyser et explorer les nouvelles données de la CACPL</v>
+        <v>Interpréter l'adéquation entre collecteurs et chiffres SIRENE de l'INSEE</v>
       </c>
       <c r="C68" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D68" s="14"/>
       <c r="E68" s="14"/>
@@ -12968,17 +13127,17 @@
       <c r="H68" s="1"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="8">
+      <c r="A69">
         <f>TachesBonus[[#This Row],[N°]]</f>
         <v>64</v>
       </c>
       <c r="B69" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Adapter le dictionnaire aux nouvelles données de la CACPL</v>
+        <v>Analyser et explorer les nouvelles données de la CACPL</v>
       </c>
       <c r="C69" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D69" s="14"/>
       <c r="E69" s="14"/>
@@ -12999,7 +13158,7 @@
       </c>
       <c r="B70" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Adapter le MCD avec les nouvelles données de la CACPL</v>
+        <v>Adapter le dictionnaire aux nouvelles données de la CACPL</v>
       </c>
       <c r="C70" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -13024,7 +13183,7 @@
       </c>
       <c r="B71" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Adapter le MLD avec les nouvelles données de la CACPL</v>
+        <v>Adapter le MCD avec les nouvelles données de la CACPL</v>
       </c>
       <c r="C71" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -13049,7 +13208,7 @@
       </c>
       <c r="B72" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Adapter le MRD avec les données de l'INSEE</v>
+        <v>Adapter le MLD avec les nouvelles données de la CACPL</v>
       </c>
       <c r="C72" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -13074,11 +13233,11 @@
       </c>
       <c r="B73" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Compléter la base de données avec les tables pour l'INSEE</v>
+        <v>Adapter le MRD avec les données de l'INSEE</v>
       </c>
       <c r="C73" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D73" s="14"/>
       <c r="E73" s="14"/>
@@ -13099,7 +13258,7 @@
       </c>
       <c r="B74" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Détecter les anomalies et nettoyer les nouvelles données de la CACPL</v>
+        <v>Compléter la base de données avec les tables pour l'INSEE</v>
       </c>
       <c r="C74" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -13124,7 +13283,7 @@
       </c>
       <c r="B75" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Mettre en forme les nouvelles données de la CACPL</v>
+        <v>Détecter les anomalies et nettoyer les nouvelles données de la CACPL</v>
       </c>
       <c r="C75" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -13149,7 +13308,7 @@
       </c>
       <c r="B76" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Intégrer dans la base de données les nouvelles données de la CACPL</v>
+        <v>Mettre en forme les nouvelles données de la CACPL</v>
       </c>
       <c r="C76" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -13174,11 +13333,11 @@
       </c>
       <c r="B77" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Créer des requêtes (CRUD) pour les nouvelles données de la CACPL</v>
+        <v>Intégrer dans la base de données les nouvelles données de la CACPL</v>
       </c>
       <c r="C77" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D77" s="14"/>
       <c r="E77" s="14"/>
@@ -13199,11 +13358,11 @@
       </c>
       <c r="B78" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Créer les graphiques croisant les données actuelles et les nouvelles de la CACPL</v>
+        <v>Créer des requêtes (CRUD) pour les nouvelles données de la CACPL</v>
       </c>
       <c r="C78" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D78" s="14"/>
       <c r="E78" s="14"/>
@@ -13224,11 +13383,11 @@
       </c>
       <c r="B79" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Intégrer les nouveaux graphiques croisés de la CACPL dans le tableau de bord</v>
+        <v>Créer les graphiques croisant les données actuelles et les nouvelles de la CACPL</v>
       </c>
       <c r="C79" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="D79" s="14"/>
       <c r="E79" s="14"/>
@@ -13249,11 +13408,11 @@
       </c>
       <c r="B80" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Générer les nouveaux graphiques pour chaque déchèterie et chaque collecteur</v>
+        <v>Intégrer les nouveaux graphiques croisés de la CACPL dans le tableau de bord</v>
       </c>
       <c r="C80" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D80" s="14"/>
       <c r="E80" s="14"/>
@@ -13274,7 +13433,7 @@
       </c>
       <c r="B81" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Intégrer les graphiques pour chaque repère de la carte</v>
+        <v>Générer les nouveaux graphiques pour chaque déchèterie et chaque collecteur</v>
       </c>
       <c r="C81" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -13299,7 +13458,7 @@
       </c>
       <c r="B82" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Rendre dynamique les graphiques de chaque repère</v>
+        <v>Intégrer les graphiques pour chaque repère de la carte</v>
       </c>
       <c r="C82" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -13324,7 +13483,7 @@
       </c>
       <c r="B83" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Afficher sur la carte les filtres issus des nouvelles données de la CACPL</v>
+        <v>Rendre dynamique les graphiques de chaque repère</v>
       </c>
       <c r="C83" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -13349,11 +13508,11 @@
       </c>
       <c r="B84" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Interpréter l'adéquation entre collecteurs et nouvelles données de la CACPL</v>
+        <v>Afficher sur la carte les filtres issus des nouvelles données de la CACPL</v>
       </c>
       <c r="C84" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D84" s="14"/>
       <c r="E84" s="14"/>
@@ -13374,11 +13533,11 @@
       </c>
       <c r="B85" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Définir les facteurs principaux d'utilsation des collecteurs</v>
+        <v>Interpréter l'adéquation entre collecteurs et nouvelles données de la CACPL</v>
       </c>
       <c r="C85" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D85" s="14"/>
       <c r="E85" s="14"/>
@@ -13399,11 +13558,11 @@
       </c>
       <c r="B86" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Définir les types d'usager</v>
+        <v>Définir les facteurs principaux d'utilsation des collecteurs</v>
       </c>
       <c r="C86" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D86" s="14"/>
       <c r="E86" s="14"/>
@@ -13424,7 +13583,7 @@
       </c>
       <c r="B87" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Définir les groupes de collecteurs</v>
+        <v>Définir les types d'usager</v>
       </c>
       <c r="C87" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -13449,11 +13608,11 @@
       </c>
       <c r="B88" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Détecter et prévoir l'utilisation des collecteurs</v>
+        <v>Définir les groupes de collecteurs</v>
       </c>
       <c r="C88" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D88" s="14"/>
       <c r="E88" s="14"/>
@@ -13474,11 +13633,11 @@
       </c>
       <c r="B89" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Transformer le tableau de bord en service</v>
+        <v>Détecter et prévoir l'utilisation des collecteurs</v>
       </c>
       <c r="C89" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D89" s="14"/>
       <c r="E89" s="14"/>
@@ -13499,7 +13658,7 @@
       </c>
       <c r="B90" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Créer une API pour le service</v>
+        <v>Transformer le tableau de bord en service</v>
       </c>
       <c r="C90" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -13524,11 +13683,11 @@
       </c>
       <c r="B91" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Afficher et rendre éditable les tables de la BDD sur le tableau de bord</v>
+        <v>Créer une API pour le service</v>
       </c>
       <c r="C91" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D91" s="14"/>
       <c r="E91" s="14"/>
@@ -13549,7 +13708,7 @@
       </c>
       <c r="B92" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v xml:space="preserve">Gérer la persistance des données éditées dans la BDD </v>
+        <v>Afficher et rendre éditable les tables de la BDD sur le tableau de bord</v>
       </c>
       <c r="C92" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -13574,11 +13733,11 @@
       </c>
       <c r="B93" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Créer le formulaire pour les comptes utilisateurs</v>
+        <v xml:space="preserve">Gérer la persistance des données éditées dans la BDD </v>
       </c>
       <c r="C93" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D93" s="14"/>
       <c r="E93" s="14"/>
@@ -13599,11 +13758,11 @@
       </c>
       <c r="B94" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v xml:space="preserve">Gérer les comptes utilisateurs </v>
+        <v>Créer le formulaire pour les comptes utilisateurs</v>
       </c>
       <c r="C94" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="D94" s="14"/>
       <c r="E94" s="14"/>
@@ -13624,7 +13783,7 @@
       </c>
       <c r="B95" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Restreindre l'accès de certaines fonctionnalités aux utilisateurs</v>
+        <v xml:space="preserve">Gérer les comptes utilisateurs </v>
       </c>
       <c r="C95" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -13649,11 +13808,11 @@
       </c>
       <c r="B96" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Créer un data lake pour tous les jeux de données</v>
+        <v>Restreindre l'accès de certaines fonctionnalités aux utilisateurs</v>
       </c>
       <c r="C96" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D96" s="14"/>
       <c r="E96" s="14"/>
@@ -13674,11 +13833,11 @@
       </c>
       <c r="B97" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Intégrer les jeux de données dans le data lake</v>
+        <v>Créer un data lake pour tous les jeux de données</v>
       </c>
       <c r="C97" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D97" s="14"/>
       <c r="E97" s="14"/>
@@ -13699,11 +13858,11 @@
       </c>
       <c r="B98" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Récupérer et éditer les informations du data lake</v>
+        <v>Intégrer les jeux de données dans le data lake</v>
       </c>
       <c r="C98" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="14"/>
@@ -13724,11 +13883,11 @@
       </c>
       <c r="B99" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Créer un exécutable</v>
+        <v>Récupérer et éditer les informations du data lake</v>
       </c>
       <c r="C99" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="D99" s="14"/>
       <c r="E99" s="14"/>
@@ -13747,13 +13906,13 @@
         <f>TachesBonus[[#This Row],[N°]]</f>
         <v>95</v>
       </c>
-      <c r="B100" s="8" t="str">
+      <c r="B100" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Se documenter sur les directives quant à la gestion des déchets</v>
+        <v>Créer un exécutable</v>
       </c>
       <c r="C100" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D100" s="14"/>
       <c r="E100" s="14"/>
@@ -13774,7 +13933,7 @@
       </c>
       <c r="B101" s="8" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Evaluer la conformité de la CACPL vis-à-vis des directives sur les déchets</v>
+        <v>Se documenter sur les directives quant à la gestion des déchets</v>
       </c>
       <c r="C101" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -13799,7 +13958,7 @@
       </c>
       <c r="B102" s="8" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Collecter les données et résultats de collecte d'autres villes</v>
+        <v>Evaluer la conformité de la CACPL vis-à-vis des directives sur les déchets</v>
       </c>
       <c r="C102" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -13824,7 +13983,7 @@
       </c>
       <c r="B103" s="8" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Comparer les dispositifs de collecte et résultats de la CACPL avec ceux d'autres villes</v>
+        <v>Collecter les données et résultats de collecte d'autres villes</v>
       </c>
       <c r="C103" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -13849,7 +14008,7 @@
       </c>
       <c r="B104" s="8" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Récupérer les données pertinentes sur le site de Météo-France</v>
+        <v>Comparer les dispositifs de collecte et résultats de la CACPL avec ceux d'autres villes</v>
       </c>
       <c r="C104" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -13874,11 +14033,11 @@
       </c>
       <c r="B105" s="8" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Détecter et prévoir l'utilisation des collecteurs selon la météo</v>
+        <v>Récupérer les données pertinentes sur le site de Météo-France</v>
       </c>
       <c r="C105" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D105" s="14"/>
       <c r="E105" s="14"/>
@@ -13899,11 +14058,11 @@
       </c>
       <c r="B106" s="8" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Récupérer les information météorologiques en continu</v>
+        <v>Détecter et prévoir l'utilisation des collecteurs selon la météo</v>
       </c>
       <c r="C106" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D106" s="14"/>
       <c r="E106" s="14"/>
@@ -13924,11 +14083,11 @@
       </c>
       <c r="B107" s="8" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Afficher sur la carte les filtres météo</v>
+        <v>Récupérer les information météorologiques en continu</v>
       </c>
       <c r="C107" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D107" s="14"/>
       <c r="E107" s="14"/>
@@ -13949,7 +14108,7 @@
       </c>
       <c r="B108" s="8" t="str">
         <f>TachesBonus[[#This Row],[Tâche]]</f>
-        <v>Actualiser les prévisions de collecte sur la carte selon la météo</v>
+        <v>Afficher sur la carte les filtres météo</v>
       </c>
       <c r="C108" s="14">
         <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
@@ -13968,13 +14127,28 @@
       <c r="H108" s="1"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A109" s="8"/>
-      <c r="B109" s="8"/>
-      <c r="C109" s="14"/>
-      <c r="D109" s="2"/>
-      <c r="E109" s="2"/>
-      <c r="F109" s="53"/>
-      <c r="G109" s="2"/>
+      <c r="A109" s="8">
+        <f>TachesBonus[[#This Row],[N°]]</f>
+        <v>104</v>
+      </c>
+      <c r="B109" s="8" t="str">
+        <f>TachesBonus[[#This Row],[Tâche]]</f>
+        <v>Actualiser les prévisions de collecte sur la carte selon la météo</v>
+      </c>
+      <c r="C109" s="14">
+        <f>TachesBonus[[#This Row],[Travail (en jours-hommes)]]</f>
+        <v>1</v>
+      </c>
+      <c r="D109" s="14"/>
+      <c r="E109" s="14"/>
+      <c r="F109" s="53">
+        <f>IFERROR(AvancementPrincipal8[[#This Row],[Temps consacré (jours-hommes)]]/(AvancementPrincipal8[[#This Row],[Temps consacré (jours-hommes)]]+AvancementPrincipal8[[#This Row],[Temps restant (jours-hommes)]]), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G109" s="14" t="str">
+        <f>IF(AvancementPrincipal8[[#This Row],[Temps consacré (jours-hommes)]]&lt;&gt;"",AvancementPrincipal8[[#This Row],[Durée estimée (jours-hommes)]]-AvancementPrincipal8[[#This Row],[Temps consacré (jours-hommes)]]-AvancementPrincipal8[[#This Row],[Temps restant (jours-hommes)]],"")</f>
+        <v/>
+      </c>
       <c r="H109" s="1"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -14026,6 +14200,16 @@
       <c r="F114" s="53"/>
       <c r="G114" s="2"/>
       <c r="H114" s="1"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" s="8"/>
+      <c r="B115" s="8"/>
+      <c r="C115" s="14"/>
+      <c r="D115" s="2"/>
+      <c r="E115" s="2"/>
+      <c r="F115" s="53"/>
+      <c r="G115" s="2"/>
+      <c r="H115" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -14049,12 +14233,12 @@
     <cfRule type="iconSet" priority="3">
       <iconSet iconSet="3Arrows">
         <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="0" gte="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F53:F108">
+  <conditionalFormatting sqref="F53:F109">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -14066,12 +14250,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G53:G108">
+  <conditionalFormatting sqref="G53:G109">
     <cfRule type="iconSet" priority="1">
       <iconSet iconSet="3Arrows">
         <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="0" gte="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
       </iconSet>
     </cfRule>
   </conditionalFormatting>

</xml_diff>